<commit_message>
Social Media Integration without Twitter
</commit_message>
<xml_diff>
--- a/Resources/Templates/Worksheets/Strategy Assessment.xlsx
+++ b/Resources/Templates/Worksheets/Strategy Assessment.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\mci\Resources\Assessments\1\xlsx\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="28800" windowHeight="16500" tabRatio="754" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16500" tabRatio="754" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1 Overall strategy" sheetId="9" r:id="rId1"/>
@@ -20,7 +15,7 @@
     <sheet name="5 Summary" sheetId="3" r:id="rId5"/>
     <sheet name="6 Data for upload" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1496,7 +1491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:T122"/>
@@ -1505,21 +1500,21 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="2" width="112.125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="112.1640625" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" style="3"/>
-    <col min="5" max="5" width="44.375" style="56" customWidth="1"/>
-    <col min="6" max="6" width="27.875" style="48" customWidth="1"/>
-    <col min="7" max="7" width="24.375" style="48" customWidth="1"/>
-    <col min="8" max="8" width="16.375" style="48" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" style="56" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" style="48" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" style="48" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" s="32" t="s">
         <v>35</v>
       </c>
@@ -1532,7 +1527,7 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:8" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="14" customFormat="1" ht="30">
       <c r="B2" s="36" t="s">
         <v>59</v>
       </c>
@@ -1555,7 +1550,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="43" t="s">
         <v>97</v>
       </c>
@@ -1566,11 +1561,11 @@
       <c r="G3" s="48"/>
       <c r="H3" s="48"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="24"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="70" t="s">
         <v>0</v>
       </c>
@@ -1592,7 +1587,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="70"/>
       <c r="B6" s="15" t="s">
         <v>34</v>
@@ -1612,7 +1607,7 @@
         <v>Identify KPIs for tracking the success of your digital communications. Ensure these are based on business objectives and are specific, measurable, attainable, realistic and time-bound (SMART goals).</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="70"/>
       <c r="B7" s="16" t="s">
         <v>9</v>
@@ -1638,7 +1633,7 @@
         <v>Identify KPIs for tracking the success of your digital communications. Ensure these are based on business objectives and are specific, measurable, attainable, realistic and time-bound (SMART goals).</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="28"/>
       <c r="B8" s="31"/>
       <c r="C8" s="45"/>
@@ -1648,7 +1643,7 @@
       <c r="G8" s="47"/>
       <c r="H8" s="47"/>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="70" t="s">
         <v>12</v>
       </c>
@@ -1670,7 +1665,7 @@
         <v>Identify specific target audience groups that are relevant to your organisation and digital communications beyond just “general population” or “all Singaporeans”.</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="70"/>
       <c r="B10" s="27" t="s">
         <v>38</v>
@@ -1690,7 +1685,7 @@
         <v>Recognise the differences in the needs, behaviour and objectives of your different audience groups and plan for how you will communicate with each group differently.</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="70"/>
       <c r="B11" s="20" t="s">
         <v>13</v>
@@ -1716,11 +1711,11 @@
         <v>Identify specific target audience groups that are relevant to your organisation and digital communications beyond just “general population” or “all Singaporeans”.Recognise the differences in the needs, behaviour and objectives of your different audience groups and plan for how you will communicate with each group differently.</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="70" t="s">
         <v>23</v>
       </c>
@@ -1742,7 +1737,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="70"/>
       <c r="B14" s="34" t="s">
         <v>57</v>
@@ -1762,7 +1757,7 @@
         <v>Assess and document your approach to amplifying your digital content through paid media (including online and traditional mass media advertising spend) as cross-promotion for your digital content.</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="70"/>
       <c r="B15" s="15" t="s">
         <v>58</v>
@@ -1782,7 +1777,7 @@
         <v>Assess and document your approach to amplifying your digital content through cultivating an influencer community by earning organic marketing through earned media optimisation.</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="70"/>
       <c r="B16" s="16" t="s">
         <v>24</v>
@@ -1808,8 +1803,8 @@
         <v>Assess and document your approach to amplifying your digital content through paid media (including online and traditional mass media advertising spend) as cross-promotion for your digital content.Assess and document your approach to amplifying your digital content through cultivating an influencer community by earning organic marketing through earned media optimisation.</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="15" customHeight="1"/>
+    <row r="18" spans="1:20" ht="15" customHeight="1">
       <c r="A18" s="70" t="s">
         <v>4</v>
       </c>
@@ -1831,7 +1826,7 @@
         <v>Identify that analytics are being monitored or tracked either via Google Analytics or other tracking tools on digital communications channels.</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="15" customHeight="1">
       <c r="A19" s="70"/>
       <c r="B19" s="15" t="s">
         <v>43</v>
@@ -1851,7 +1846,7 @@
         <v>Define the process of improving digital performance on communications channels using data from analytics tools.</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="15" customHeight="1">
       <c r="A20" s="70"/>
       <c r="B20" s="16" t="s">
         <v>15</v>
@@ -1877,10 +1872,10 @@
         <v>Identify that analytics are being monitored or tracked either via Google Analytics or other tracking tools on digital communications channels.Define the process of improving digital performance on communications channels using data from analytics tools.</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15" customHeight="1">
       <c r="E21" s="59"/>
     </row>
-    <row r="22" spans="1:20" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="70" t="s">
         <v>54</v>
       </c>
@@ -1915,7 +1910,7 @@
       <c r="S22"/>
       <c r="T22"/>
     </row>
-    <row r="23" spans="1:20" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="A23" s="70"/>
       <c r="B23" s="16" t="s">
         <v>61</v>
@@ -1954,7 +1949,7 @@
       <c r="S23"/>
       <c r="T23"/>
     </row>
-    <row r="24" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" s="11" customFormat="1">
       <c r="A24"/>
       <c r="B24" s="23"/>
       <c r="C24" s="3"/>
@@ -1976,7 +1971,7 @@
       <c r="S24"/>
       <c r="T24"/>
     </row>
-    <row r="25" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="11" customFormat="1">
       <c r="A25"/>
       <c r="B25" s="23"/>
       <c r="C25" s="3"/>
@@ -1998,7 +1993,7 @@
       <c r="S25"/>
       <c r="T25"/>
     </row>
-    <row r="26" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="11" customFormat="1">
       <c r="A26"/>
       <c r="B26" s="23"/>
       <c r="C26" s="3"/>
@@ -2020,7 +2015,7 @@
       <c r="S26"/>
       <c r="T26"/>
     </row>
-    <row r="27" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="11" customFormat="1">
       <c r="A27"/>
       <c r="B27" s="23"/>
       <c r="C27" s="3"/>
@@ -2042,7 +2037,7 @@
       <c r="S27"/>
       <c r="T27"/>
     </row>
-    <row r="28" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" s="11" customFormat="1">
       <c r="A28"/>
       <c r="B28" s="23"/>
       <c r="C28" s="3"/>
@@ -2064,7 +2059,7 @@
       <c r="S28"/>
       <c r="T28"/>
     </row>
-    <row r="29" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" s="11" customFormat="1">
       <c r="A29"/>
       <c r="B29" s="23"/>
       <c r="C29" s="3"/>
@@ -2086,7 +2081,7 @@
       <c r="S29"/>
       <c r="T29"/>
     </row>
-    <row r="30" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" s="11" customFormat="1">
       <c r="A30"/>
       <c r="B30" s="23"/>
       <c r="C30" s="3"/>
@@ -2108,7 +2103,7 @@
       <c r="S30"/>
       <c r="T30"/>
     </row>
-    <row r="31" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" s="11" customFormat="1">
       <c r="A31"/>
       <c r="B31" s="23"/>
       <c r="C31" s="3"/>
@@ -2130,7 +2125,7 @@
       <c r="S31"/>
       <c r="T31"/>
     </row>
-    <row r="32" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" s="11" customFormat="1">
       <c r="A32"/>
       <c r="B32" s="23"/>
       <c r="C32" s="3"/>
@@ -2152,7 +2147,7 @@
       <c r="S32"/>
       <c r="T32"/>
     </row>
-    <row r="33" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" s="11" customFormat="1">
       <c r="A33"/>
       <c r="B33" s="23"/>
       <c r="C33" s="3"/>
@@ -2174,7 +2169,7 @@
       <c r="S33"/>
       <c r="T33"/>
     </row>
-    <row r="34" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" s="11" customFormat="1">
       <c r="A34"/>
       <c r="B34" s="23"/>
       <c r="C34" s="3"/>
@@ -2196,7 +2191,7 @@
       <c r="S34"/>
       <c r="T34"/>
     </row>
-    <row r="35" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" s="11" customFormat="1">
       <c r="A35"/>
       <c r="B35" s="23"/>
       <c r="C35" s="3"/>
@@ -2218,7 +2213,7 @@
       <c r="S35"/>
       <c r="T35"/>
     </row>
-    <row r="36" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" s="11" customFormat="1">
       <c r="A36"/>
       <c r="B36" s="23"/>
       <c r="C36" s="3"/>
@@ -2240,7 +2235,7 @@
       <c r="S36"/>
       <c r="T36"/>
     </row>
-    <row r="37" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" s="11" customFormat="1">
       <c r="A37"/>
       <c r="B37" s="23"/>
       <c r="C37" s="3"/>
@@ -2262,7 +2257,7 @@
       <c r="S37"/>
       <c r="T37"/>
     </row>
-    <row r="38" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" s="11" customFormat="1">
       <c r="A38"/>
       <c r="B38" s="23"/>
       <c r="C38" s="3"/>
@@ -2284,7 +2279,7 @@
       <c r="S38"/>
       <c r="T38"/>
     </row>
-    <row r="39" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" s="11" customFormat="1">
       <c r="A39"/>
       <c r="B39" s="23"/>
       <c r="C39" s="3"/>
@@ -2306,7 +2301,7 @@
       <c r="S39"/>
       <c r="T39"/>
     </row>
-    <row r="40" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" s="11" customFormat="1">
       <c r="A40"/>
       <c r="B40" s="23"/>
       <c r="C40" s="3"/>
@@ -2328,7 +2323,7 @@
       <c r="S40"/>
       <c r="T40"/>
     </row>
-    <row r="41" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" s="11" customFormat="1">
       <c r="A41"/>
       <c r="B41" s="23"/>
       <c r="C41" s="3"/>
@@ -2350,7 +2345,7 @@
       <c r="S41"/>
       <c r="T41"/>
     </row>
-    <row r="42" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" s="11" customFormat="1">
       <c r="A42"/>
       <c r="B42" s="23"/>
       <c r="C42" s="3"/>
@@ -2372,7 +2367,7 @@
       <c r="S42"/>
       <c r="T42"/>
     </row>
-    <row r="43" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" s="11" customFormat="1">
       <c r="A43"/>
       <c r="B43" s="23"/>
       <c r="C43" s="3"/>
@@ -2394,7 +2389,7 @@
       <c r="S43"/>
       <c r="T43"/>
     </row>
-    <row r="44" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" s="11" customFormat="1">
       <c r="A44"/>
       <c r="B44" s="23"/>
       <c r="C44" s="3"/>
@@ -2416,7 +2411,7 @@
       <c r="S44"/>
       <c r="T44"/>
     </row>
-    <row r="45" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" s="11" customFormat="1">
       <c r="A45"/>
       <c r="B45" s="23"/>
       <c r="C45" s="3"/>
@@ -2438,7 +2433,7 @@
       <c r="S45"/>
       <c r="T45"/>
     </row>
-    <row r="46" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" s="11" customFormat="1">
       <c r="A46"/>
       <c r="B46" s="23"/>
       <c r="C46" s="3"/>
@@ -2460,7 +2455,7 @@
       <c r="S46"/>
       <c r="T46"/>
     </row>
-    <row r="47" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" s="11" customFormat="1">
       <c r="A47"/>
       <c r="B47" s="23"/>
       <c r="C47" s="3"/>
@@ -2482,7 +2477,7 @@
       <c r="S47"/>
       <c r="T47"/>
     </row>
-    <row r="48" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" s="11" customFormat="1">
       <c r="A48"/>
       <c r="B48" s="23"/>
       <c r="C48" s="3"/>
@@ -2504,7 +2499,7 @@
       <c r="S48"/>
       <c r="T48"/>
     </row>
-    <row r="49" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" s="11" customFormat="1">
       <c r="A49"/>
       <c r="B49" s="23"/>
       <c r="C49" s="3"/>
@@ -2526,7 +2521,7 @@
       <c r="S49"/>
       <c r="T49"/>
     </row>
-    <row r="50" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" s="11" customFormat="1">
       <c r="A50"/>
       <c r="B50" s="23"/>
       <c r="C50" s="3"/>
@@ -2548,7 +2543,7 @@
       <c r="S50"/>
       <c r="T50"/>
     </row>
-    <row r="51" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" s="11" customFormat="1">
       <c r="A51"/>
       <c r="B51" s="23"/>
       <c r="C51" s="3"/>
@@ -2570,7 +2565,7 @@
       <c r="S51"/>
       <c r="T51"/>
     </row>
-    <row r="52" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" s="11" customFormat="1">
       <c r="A52"/>
       <c r="B52" s="23"/>
       <c r="C52" s="3"/>
@@ -2592,7 +2587,7 @@
       <c r="S52"/>
       <c r="T52"/>
     </row>
-    <row r="53" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" s="11" customFormat="1">
       <c r="A53"/>
       <c r="B53" s="23"/>
       <c r="C53" s="3"/>
@@ -2614,7 +2609,7 @@
       <c r="S53"/>
       <c r="T53"/>
     </row>
-    <row r="54" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" s="11" customFormat="1">
       <c r="A54"/>
       <c r="B54" s="23"/>
       <c r="C54" s="3"/>
@@ -2636,7 +2631,7 @@
       <c r="S54"/>
       <c r="T54"/>
     </row>
-    <row r="55" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" s="11" customFormat="1">
       <c r="A55"/>
       <c r="B55" s="23"/>
       <c r="C55" s="3"/>
@@ -2658,7 +2653,7 @@
       <c r="S55"/>
       <c r="T55"/>
     </row>
-    <row r="56" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" s="11" customFormat="1">
       <c r="A56"/>
       <c r="B56" s="23"/>
       <c r="C56" s="3"/>
@@ -2680,7 +2675,7 @@
       <c r="S56"/>
       <c r="T56"/>
     </row>
-    <row r="57" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" s="11" customFormat="1">
       <c r="A57"/>
       <c r="B57" s="23"/>
       <c r="C57" s="3"/>
@@ -2702,7 +2697,7 @@
       <c r="S57"/>
       <c r="T57"/>
     </row>
-    <row r="58" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" s="11" customFormat="1">
       <c r="A58"/>
       <c r="B58" s="23"/>
       <c r="C58" s="3"/>
@@ -2724,7 +2719,7 @@
       <c r="S58"/>
       <c r="T58"/>
     </row>
-    <row r="59" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" s="11" customFormat="1">
       <c r="A59"/>
       <c r="B59" s="23"/>
       <c r="C59" s="3"/>
@@ -2746,7 +2741,7 @@
       <c r="S59"/>
       <c r="T59"/>
     </row>
-    <row r="60" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" s="11" customFormat="1">
       <c r="A60"/>
       <c r="B60" s="23"/>
       <c r="C60" s="3"/>
@@ -2768,7 +2763,7 @@
       <c r="S60"/>
       <c r="T60"/>
     </row>
-    <row r="61" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" s="11" customFormat="1">
       <c r="A61"/>
       <c r="B61" s="23"/>
       <c r="C61" s="3"/>
@@ -2790,7 +2785,7 @@
       <c r="S61"/>
       <c r="T61"/>
     </row>
-    <row r="62" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" s="11" customFormat="1">
       <c r="A62"/>
       <c r="B62" s="23"/>
       <c r="C62" s="3"/>
@@ -2812,7 +2807,7 @@
       <c r="S62"/>
       <c r="T62"/>
     </row>
-    <row r="63" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" s="11" customFormat="1">
       <c r="A63"/>
       <c r="B63" s="23"/>
       <c r="C63" s="3"/>
@@ -2834,7 +2829,7 @@
       <c r="S63"/>
       <c r="T63"/>
     </row>
-    <row r="64" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" s="11" customFormat="1">
       <c r="A64"/>
       <c r="B64" s="23"/>
       <c r="C64" s="3"/>
@@ -2856,7 +2851,7 @@
       <c r="S64"/>
       <c r="T64"/>
     </row>
-    <row r="65" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" s="11" customFormat="1">
       <c r="A65"/>
       <c r="B65" s="23"/>
       <c r="C65" s="3"/>
@@ -2878,7 +2873,7 @@
       <c r="S65"/>
       <c r="T65"/>
     </row>
-    <row r="66" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" s="11" customFormat="1">
       <c r="A66"/>
       <c r="B66" s="23"/>
       <c r="C66" s="3"/>
@@ -2900,7 +2895,7 @@
       <c r="S66"/>
       <c r="T66"/>
     </row>
-    <row r="67" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" s="11" customFormat="1">
       <c r="A67"/>
       <c r="B67" s="23"/>
       <c r="C67" s="3"/>
@@ -2922,7 +2917,7 @@
       <c r="S67"/>
       <c r="T67"/>
     </row>
-    <row r="68" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" s="11" customFormat="1">
       <c r="A68"/>
       <c r="B68" s="23"/>
       <c r="C68" s="3"/>
@@ -2944,7 +2939,7 @@
       <c r="S68"/>
       <c r="T68"/>
     </row>
-    <row r="69" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" s="11" customFormat="1">
       <c r="A69"/>
       <c r="B69" s="23"/>
       <c r="C69" s="3"/>
@@ -2966,7 +2961,7 @@
       <c r="S69"/>
       <c r="T69"/>
     </row>
-    <row r="70" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" s="11" customFormat="1">
       <c r="A70"/>
       <c r="B70" s="23"/>
       <c r="C70" s="3"/>
@@ -2988,7 +2983,7 @@
       <c r="S70"/>
       <c r="T70"/>
     </row>
-    <row r="71" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" s="11" customFormat="1">
       <c r="A71"/>
       <c r="B71" s="23"/>
       <c r="C71" s="3"/>
@@ -3010,7 +3005,7 @@
       <c r="S71"/>
       <c r="T71"/>
     </row>
-    <row r="72" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" s="11" customFormat="1">
       <c r="A72"/>
       <c r="B72" s="23"/>
       <c r="C72" s="3"/>
@@ -3032,7 +3027,7 @@
       <c r="S72"/>
       <c r="T72"/>
     </row>
-    <row r="73" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" s="11" customFormat="1">
       <c r="A73"/>
       <c r="B73" s="23"/>
       <c r="C73" s="3"/>
@@ -3054,7 +3049,7 @@
       <c r="S73"/>
       <c r="T73"/>
     </row>
-    <row r="74" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" s="11" customFormat="1">
       <c r="A74"/>
       <c r="B74" s="23"/>
       <c r="C74" s="3"/>
@@ -3076,7 +3071,7 @@
       <c r="S74"/>
       <c r="T74"/>
     </row>
-    <row r="75" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" s="11" customFormat="1">
       <c r="A75"/>
       <c r="B75" s="23"/>
       <c r="C75" s="3"/>
@@ -3098,7 +3093,7 @@
       <c r="S75"/>
       <c r="T75"/>
     </row>
-    <row r="76" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" s="11" customFormat="1">
       <c r="A76"/>
       <c r="B76" s="23"/>
       <c r="C76" s="3"/>
@@ -3120,7 +3115,7 @@
       <c r="S76"/>
       <c r="T76"/>
     </row>
-    <row r="77" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" s="11" customFormat="1">
       <c r="A77"/>
       <c r="B77" s="23"/>
       <c r="C77" s="3"/>
@@ -3142,7 +3137,7 @@
       <c r="S77"/>
       <c r="T77"/>
     </row>
-    <row r="78" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" s="11" customFormat="1">
       <c r="A78"/>
       <c r="B78" s="23"/>
       <c r="C78" s="3"/>
@@ -3164,7 +3159,7 @@
       <c r="S78"/>
       <c r="T78"/>
     </row>
-    <row r="79" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" s="11" customFormat="1">
       <c r="A79"/>
       <c r="B79" s="23"/>
       <c r="C79" s="3"/>
@@ -3186,7 +3181,7 @@
       <c r="S79"/>
       <c r="T79"/>
     </row>
-    <row r="80" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" s="11" customFormat="1">
       <c r="A80"/>
       <c r="B80" s="23"/>
       <c r="C80" s="3"/>
@@ -3208,7 +3203,7 @@
       <c r="S80"/>
       <c r="T80"/>
     </row>
-    <row r="81" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" s="11" customFormat="1">
       <c r="A81"/>
       <c r="B81" s="23"/>
       <c r="C81" s="3"/>
@@ -3230,7 +3225,7 @@
       <c r="S81"/>
       <c r="T81"/>
     </row>
-    <row r="82" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" s="11" customFormat="1">
       <c r="A82"/>
       <c r="B82" s="23"/>
       <c r="C82" s="3"/>
@@ -3252,7 +3247,7 @@
       <c r="S82"/>
       <c r="T82"/>
     </row>
-    <row r="83" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" s="11" customFormat="1">
       <c r="A83"/>
       <c r="B83" s="23"/>
       <c r="C83" s="3"/>
@@ -3274,7 +3269,7 @@
       <c r="S83"/>
       <c r="T83"/>
     </row>
-    <row r="84" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" s="11" customFormat="1">
       <c r="A84"/>
       <c r="B84" s="23"/>
       <c r="C84" s="3"/>
@@ -3296,7 +3291,7 @@
       <c r="S84"/>
       <c r="T84"/>
     </row>
-    <row r="85" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" s="11" customFormat="1">
       <c r="A85"/>
       <c r="B85" s="23"/>
       <c r="C85" s="3"/>
@@ -3318,7 +3313,7 @@
       <c r="S85"/>
       <c r="T85"/>
     </row>
-    <row r="86" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" s="11" customFormat="1">
       <c r="A86"/>
       <c r="B86" s="23"/>
       <c r="C86" s="3"/>
@@ -3340,7 +3335,7 @@
       <c r="S86"/>
       <c r="T86"/>
     </row>
-    <row r="87" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" s="11" customFormat="1">
       <c r="A87"/>
       <c r="B87" s="23"/>
       <c r="C87" s="3"/>
@@ -3362,7 +3357,7 @@
       <c r="S87"/>
       <c r="T87"/>
     </row>
-    <row r="88" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" s="11" customFormat="1">
       <c r="A88"/>
       <c r="B88" s="23"/>
       <c r="C88" s="3"/>
@@ -3384,7 +3379,7 @@
       <c r="S88"/>
       <c r="T88"/>
     </row>
-    <row r="89" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" s="11" customFormat="1">
       <c r="A89"/>
       <c r="B89" s="23"/>
       <c r="C89" s="3"/>
@@ -3406,7 +3401,7 @@
       <c r="S89"/>
       <c r="T89"/>
     </row>
-    <row r="90" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" s="11" customFormat="1">
       <c r="A90"/>
       <c r="B90" s="23"/>
       <c r="C90" s="3"/>
@@ -3428,7 +3423,7 @@
       <c r="S90"/>
       <c r="T90"/>
     </row>
-    <row r="91" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" s="11" customFormat="1">
       <c r="A91"/>
       <c r="B91" s="23"/>
       <c r="C91" s="3"/>
@@ -3450,7 +3445,7 @@
       <c r="S91"/>
       <c r="T91"/>
     </row>
-    <row r="92" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" s="11" customFormat="1">
       <c r="A92"/>
       <c r="B92" s="23"/>
       <c r="C92" s="3"/>
@@ -3472,7 +3467,7 @@
       <c r="S92"/>
       <c r="T92"/>
     </row>
-    <row r="93" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" s="11" customFormat="1">
       <c r="A93"/>
       <c r="B93" s="23"/>
       <c r="C93" s="3"/>
@@ -3494,7 +3489,7 @@
       <c r="S93"/>
       <c r="T93"/>
     </row>
-    <row r="94" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" s="11" customFormat="1">
       <c r="A94"/>
       <c r="B94" s="23"/>
       <c r="C94" s="3"/>
@@ -3516,7 +3511,7 @@
       <c r="S94"/>
       <c r="T94"/>
     </row>
-    <row r="95" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" s="11" customFormat="1">
       <c r="A95"/>
       <c r="B95" s="23"/>
       <c r="C95" s="3"/>
@@ -3538,7 +3533,7 @@
       <c r="S95"/>
       <c r="T95"/>
     </row>
-    <row r="96" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" s="11" customFormat="1">
       <c r="A96"/>
       <c r="B96" s="23"/>
       <c r="C96" s="3"/>
@@ -3560,7 +3555,7 @@
       <c r="S96"/>
       <c r="T96"/>
     </row>
-    <row r="97" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" s="11" customFormat="1">
       <c r="A97"/>
       <c r="B97" s="23"/>
       <c r="C97" s="3"/>
@@ -3582,7 +3577,7 @@
       <c r="S97"/>
       <c r="T97"/>
     </row>
-    <row r="98" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" s="11" customFormat="1">
       <c r="A98"/>
       <c r="B98" s="23"/>
       <c r="C98" s="3"/>
@@ -3604,7 +3599,7 @@
       <c r="S98"/>
       <c r="T98"/>
     </row>
-    <row r="99" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" s="11" customFormat="1">
       <c r="A99"/>
       <c r="B99" s="23"/>
       <c r="C99" s="3"/>
@@ -3626,7 +3621,7 @@
       <c r="S99"/>
       <c r="T99"/>
     </row>
-    <row r="100" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" s="11" customFormat="1">
       <c r="A100"/>
       <c r="B100" s="23"/>
       <c r="C100" s="3"/>
@@ -3648,7 +3643,7 @@
       <c r="S100"/>
       <c r="T100"/>
     </row>
-    <row r="101" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" s="11" customFormat="1">
       <c r="A101"/>
       <c r="B101" s="23"/>
       <c r="C101" s="3"/>
@@ -3670,7 +3665,7 @@
       <c r="S101"/>
       <c r="T101"/>
     </row>
-    <row r="102" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" s="11" customFormat="1">
       <c r="A102"/>
       <c r="B102" s="23"/>
       <c r="C102" s="3"/>
@@ -3692,7 +3687,7 @@
       <c r="S102"/>
       <c r="T102"/>
     </row>
-    <row r="103" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" s="11" customFormat="1">
       <c r="A103"/>
       <c r="B103" s="23"/>
       <c r="C103" s="3"/>
@@ -3714,7 +3709,7 @@
       <c r="S103"/>
       <c r="T103"/>
     </row>
-    <row r="104" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" s="11" customFormat="1">
       <c r="A104"/>
       <c r="B104" s="23"/>
       <c r="C104" s="3"/>
@@ -3736,7 +3731,7 @@
       <c r="S104"/>
       <c r="T104"/>
     </row>
-    <row r="105" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" s="11" customFormat="1">
       <c r="A105"/>
       <c r="B105" s="23"/>
       <c r="C105" s="3"/>
@@ -3758,7 +3753,7 @@
       <c r="S105"/>
       <c r="T105"/>
     </row>
-    <row r="106" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" s="11" customFormat="1">
       <c r="A106"/>
       <c r="B106" s="23"/>
       <c r="C106" s="3"/>
@@ -3780,7 +3775,7 @@
       <c r="S106"/>
       <c r="T106"/>
     </row>
-    <row r="107" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" s="11" customFormat="1">
       <c r="A107"/>
       <c r="B107" s="23"/>
       <c r="C107" s="3"/>
@@ -3802,7 +3797,7 @@
       <c r="S107"/>
       <c r="T107"/>
     </row>
-    <row r="108" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" s="11" customFormat="1">
       <c r="A108"/>
       <c r="B108" s="23"/>
       <c r="C108" s="3"/>
@@ -3824,7 +3819,7 @@
       <c r="S108"/>
       <c r="T108"/>
     </row>
-    <row r="109" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" s="11" customFormat="1">
       <c r="A109"/>
       <c r="B109" s="23"/>
       <c r="C109" s="3"/>
@@ -3846,7 +3841,7 @@
       <c r="S109"/>
       <c r="T109"/>
     </row>
-    <row r="110" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" s="11" customFormat="1">
       <c r="A110"/>
       <c r="B110" s="23"/>
       <c r="C110" s="3"/>
@@ -3868,7 +3863,7 @@
       <c r="S110"/>
       <c r="T110"/>
     </row>
-    <row r="111" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" s="11" customFormat="1">
       <c r="A111"/>
       <c r="B111" s="23"/>
       <c r="C111" s="3"/>
@@ -3890,7 +3885,7 @@
       <c r="S111"/>
       <c r="T111"/>
     </row>
-    <row r="112" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" s="11" customFormat="1">
       <c r="A112"/>
       <c r="B112" s="23"/>
       <c r="C112" s="3"/>
@@ -3912,7 +3907,7 @@
       <c r="S112"/>
       <c r="T112"/>
     </row>
-    <row r="113" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" s="11" customFormat="1">
       <c r="A113"/>
       <c r="B113" s="23"/>
       <c r="C113" s="3"/>
@@ -3934,7 +3929,7 @@
       <c r="S113"/>
       <c r="T113"/>
     </row>
-    <row r="114" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" s="11" customFormat="1">
       <c r="A114"/>
       <c r="B114" s="23"/>
       <c r="C114" s="3"/>
@@ -3956,7 +3951,7 @@
       <c r="S114"/>
       <c r="T114"/>
     </row>
-    <row r="115" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" s="11" customFormat="1">
       <c r="A115"/>
       <c r="B115" s="23"/>
       <c r="C115" s="3"/>
@@ -3978,7 +3973,7 @@
       <c r="S115"/>
       <c r="T115"/>
     </row>
-    <row r="116" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" s="11" customFormat="1">
       <c r="A116"/>
       <c r="B116" s="23"/>
       <c r="C116" s="3"/>
@@ -4000,7 +3995,7 @@
       <c r="S116"/>
       <c r="T116"/>
     </row>
-    <row r="117" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" s="11" customFormat="1">
       <c r="A117"/>
       <c r="B117" s="23"/>
       <c r="C117" s="3"/>
@@ -4022,7 +4017,7 @@
       <c r="S117"/>
       <c r="T117"/>
     </row>
-    <row r="118" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" s="11" customFormat="1">
       <c r="A118"/>
       <c r="B118" s="23"/>
       <c r="C118" s="3"/>
@@ -4044,7 +4039,7 @@
       <c r="S118"/>
       <c r="T118"/>
     </row>
-    <row r="119" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" s="11" customFormat="1">
       <c r="A119"/>
       <c r="B119" s="23"/>
       <c r="C119" s="3"/>
@@ -4066,7 +4061,7 @@
       <c r="S119"/>
       <c r="T119"/>
     </row>
-    <row r="120" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" s="11" customFormat="1">
       <c r="A120"/>
       <c r="B120" s="23"/>
       <c r="C120" s="3"/>
@@ -4088,7 +4083,7 @@
       <c r="S120"/>
       <c r="T120"/>
     </row>
-    <row r="121" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" s="11" customFormat="1">
       <c r="A121"/>
       <c r="B121" s="23"/>
       <c r="C121" s="3"/>
@@ -4110,7 +4105,7 @@
       <c r="S121"/>
       <c r="T121"/>
     </row>
-    <row r="122" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" s="11" customFormat="1">
       <c r="A122"/>
       <c r="B122" s="23"/>
       <c r="C122" s="3"/>
@@ -4159,7 +4154,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:S118"/>
@@ -4169,21 +4164,21 @@
       <selection activeCell="B55" sqref="B55"/>
       <selection pane="topRight" activeCell="B55" sqref="B55"/>
       <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="2" width="79" style="23" customWidth="1"/>
     <col min="3" max="4" width="11" style="6"/>
-    <col min="5" max="5" width="44.375" customWidth="1"/>
-    <col min="6" max="6" width="27.875" customWidth="1"/>
-    <col min="7" max="7" width="24.375" customWidth="1"/>
-    <col min="8" max="8" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" s="32" t="s">
         <v>22</v>
       </c>
@@ -4196,7 +4191,7 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="30">
       <c r="B2" s="36" t="s">
         <v>8</v>
       </c>
@@ -4219,7 +4214,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="27" t="s">
         <v>127</v>
       </c>
@@ -4229,7 +4224,7 @@
       <c r="G3" s="48"/>
       <c r="H3" s="48"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="44"/>
       <c r="B4" s="24"/>
       <c r="E4" s="55"/>
@@ -4237,7 +4232,7 @@
       <c r="G4" s="48"/>
       <c r="H4" s="48"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="70" t="s">
         <v>3</v>
       </c>
@@ -4257,7 +4252,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="70"/>
       <c r="B6" s="27" t="s">
         <v>41</v>
@@ -4277,7 +4272,7 @@
         <v>Investigate and document the creation and approval workflows for content in your organisation. Include steps like sourcing, creating, editing, reviewing, approving, publishing and culling content.</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="70"/>
       <c r="B7" s="27" t="s">
         <v>42</v>
@@ -4295,7 +4290,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="70"/>
       <c r="B8" s="27" t="s">
         <v>47</v>
@@ -4315,7 +4310,7 @@
         <v>Define guidelines for the tone of voice to adopt on your website(s). Base this on your organisation’s brand guidelines, but take into account potential differences in the audiences of your online channels.</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="70"/>
       <c r="B9" s="20" t="s">
         <v>16</v>
@@ -4342,28 +4337,28 @@
         <v>Investigate and document the creation and approval workflows for content in your organisation. Include steps like sourcing, creating, editing, reviewing, approving, publishing and culling content.Define guidelines for the tone of voice to adopt on your website(s). Base this on your organisation’s brand guidelines, but take into account potential differences in the audiences of your online channels.</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="19" customFormat="1">
       <c r="A13" s="28"/>
       <c r="B13" s="29"/>
       <c r="C13" s="18"/>
       <c r="D13" s="30"/>
     </row>
-    <row r="18" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" s="11" customFormat="1">
       <c r="A18"/>
       <c r="B18" s="23"/>
       <c r="C18" s="6"/>
@@ -4384,7 +4379,7 @@
       <c r="R18"/>
       <c r="S18"/>
     </row>
-    <row r="19" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" s="11" customFormat="1">
       <c r="A19"/>
       <c r="B19" s="23"/>
       <c r="C19" s="6"/>
@@ -4405,7 +4400,7 @@
       <c r="R19"/>
       <c r="S19"/>
     </row>
-    <row r="20" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" s="11" customFormat="1">
       <c r="A20"/>
       <c r="B20" s="23"/>
       <c r="C20" s="6"/>
@@ -4426,7 +4421,7 @@
       <c r="R20"/>
       <c r="S20"/>
     </row>
-    <row r="21" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" s="11" customFormat="1">
       <c r="A21"/>
       <c r="B21" s="23"/>
       <c r="C21" s="6"/>
@@ -4447,7 +4442,7 @@
       <c r="R21"/>
       <c r="S21"/>
     </row>
-    <row r="22" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" s="11" customFormat="1">
       <c r="A22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="6"/>
@@ -4468,7 +4463,7 @@
       <c r="R22"/>
       <c r="S22"/>
     </row>
-    <row r="23" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" s="11" customFormat="1">
       <c r="A23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="6"/>
@@ -4489,7 +4484,7 @@
       <c r="R23"/>
       <c r="S23"/>
     </row>
-    <row r="24" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" s="11" customFormat="1">
       <c r="A24"/>
       <c r="B24" s="23"/>
       <c r="C24" s="6"/>
@@ -4510,7 +4505,7 @@
       <c r="R24"/>
       <c r="S24"/>
     </row>
-    <row r="25" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" s="11" customFormat="1">
       <c r="A25"/>
       <c r="B25" s="23"/>
       <c r="C25" s="6"/>
@@ -4531,7 +4526,7 @@
       <c r="R25"/>
       <c r="S25"/>
     </row>
-    <row r="26" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" s="11" customFormat="1">
       <c r="A26"/>
       <c r="B26" s="23"/>
       <c r="C26" s="6"/>
@@ -4552,7 +4547,7 @@
       <c r="R26"/>
       <c r="S26"/>
     </row>
-    <row r="27" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" s="11" customFormat="1">
       <c r="A27"/>
       <c r="B27" s="23"/>
       <c r="C27" s="6"/>
@@ -4573,7 +4568,7 @@
       <c r="R27"/>
       <c r="S27"/>
     </row>
-    <row r="28" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" s="11" customFormat="1">
       <c r="A28"/>
       <c r="B28" s="23"/>
       <c r="C28" s="6"/>
@@ -4594,7 +4589,7 @@
       <c r="R28"/>
       <c r="S28"/>
     </row>
-    <row r="29" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" s="11" customFormat="1">
       <c r="A29"/>
       <c r="B29" s="23"/>
       <c r="C29" s="6"/>
@@ -4615,7 +4610,7 @@
       <c r="R29"/>
       <c r="S29"/>
     </row>
-    <row r="30" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" s="11" customFormat="1">
       <c r="A30"/>
       <c r="B30" s="23"/>
       <c r="C30" s="6"/>
@@ -4636,7 +4631,7 @@
       <c r="R30"/>
       <c r="S30"/>
     </row>
-    <row r="31" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" s="11" customFormat="1">
       <c r="A31"/>
       <c r="B31" s="23"/>
       <c r="C31" s="6"/>
@@ -4657,7 +4652,7 @@
       <c r="R31"/>
       <c r="S31"/>
     </row>
-    <row r="32" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" s="11" customFormat="1">
       <c r="A32"/>
       <c r="B32" s="23"/>
       <c r="C32" s="6"/>
@@ -4678,7 +4673,7 @@
       <c r="R32"/>
       <c r="S32"/>
     </row>
-    <row r="33" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" s="11" customFormat="1">
       <c r="A33"/>
       <c r="B33" s="23"/>
       <c r="C33" s="6"/>
@@ -4699,7 +4694,7 @@
       <c r="R33"/>
       <c r="S33"/>
     </row>
-    <row r="34" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" s="11" customFormat="1">
       <c r="A34"/>
       <c r="B34" s="23"/>
       <c r="C34" s="6"/>
@@ -4720,7 +4715,7 @@
       <c r="R34"/>
       <c r="S34"/>
     </row>
-    <row r="35" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" s="11" customFormat="1">
       <c r="A35"/>
       <c r="B35" s="23"/>
       <c r="C35" s="6"/>
@@ -4741,7 +4736,7 @@
       <c r="R35"/>
       <c r="S35"/>
     </row>
-    <row r="36" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" s="11" customFormat="1">
       <c r="A36"/>
       <c r="B36" s="23"/>
       <c r="C36" s="6"/>
@@ -4762,7 +4757,7 @@
       <c r="R36"/>
       <c r="S36"/>
     </row>
-    <row r="37" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" s="11" customFormat="1">
       <c r="A37"/>
       <c r="B37" s="23"/>
       <c r="C37" s="6"/>
@@ -4783,7 +4778,7 @@
       <c r="R37"/>
       <c r="S37"/>
     </row>
-    <row r="38" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" s="11" customFormat="1">
       <c r="A38"/>
       <c r="B38" s="23"/>
       <c r="C38" s="6"/>
@@ -4804,7 +4799,7 @@
       <c r="R38"/>
       <c r="S38"/>
     </row>
-    <row r="39" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" s="11" customFormat="1">
       <c r="A39"/>
       <c r="B39" s="23"/>
       <c r="C39" s="6"/>
@@ -4825,7 +4820,7 @@
       <c r="R39"/>
       <c r="S39"/>
     </row>
-    <row r="40" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" s="11" customFormat="1">
       <c r="A40"/>
       <c r="B40" s="23"/>
       <c r="C40" s="6"/>
@@ -4846,7 +4841,7 @@
       <c r="R40"/>
       <c r="S40"/>
     </row>
-    <row r="41" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" s="11" customFormat="1">
       <c r="A41"/>
       <c r="B41" s="23"/>
       <c r="C41" s="6"/>
@@ -4867,7 +4862,7 @@
       <c r="R41"/>
       <c r="S41"/>
     </row>
-    <row r="42" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" s="11" customFormat="1">
       <c r="A42"/>
       <c r="B42" s="23"/>
       <c r="C42" s="6"/>
@@ -4888,7 +4883,7 @@
       <c r="R42"/>
       <c r="S42"/>
     </row>
-    <row r="43" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" s="11" customFormat="1">
       <c r="A43"/>
       <c r="B43" s="23"/>
       <c r="C43" s="6"/>
@@ -4909,7 +4904,7 @@
       <c r="R43"/>
       <c r="S43"/>
     </row>
-    <row r="44" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" s="11" customFormat="1">
       <c r="A44"/>
       <c r="B44" s="23"/>
       <c r="C44" s="6"/>
@@ -4930,7 +4925,7 @@
       <c r="R44"/>
       <c r="S44"/>
     </row>
-    <row r="45" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" s="11" customFormat="1">
       <c r="A45"/>
       <c r="B45" s="23"/>
       <c r="C45" s="6"/>
@@ -4951,7 +4946,7 @@
       <c r="R45"/>
       <c r="S45"/>
     </row>
-    <row r="46" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" s="11" customFormat="1">
       <c r="A46"/>
       <c r="B46" s="23"/>
       <c r="C46" s="6"/>
@@ -4972,7 +4967,7 @@
       <c r="R46"/>
       <c r="S46"/>
     </row>
-    <row r="47" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" s="11" customFormat="1">
       <c r="A47"/>
       <c r="B47" s="23"/>
       <c r="C47" s="6"/>
@@ -4993,7 +4988,7 @@
       <c r="R47"/>
       <c r="S47"/>
     </row>
-    <row r="48" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" s="11" customFormat="1">
       <c r="A48"/>
       <c r="B48" s="23"/>
       <c r="C48" s="6"/>
@@ -5014,7 +5009,7 @@
       <c r="R48"/>
       <c r="S48"/>
     </row>
-    <row r="49" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" s="11" customFormat="1">
       <c r="A49"/>
       <c r="B49" s="23"/>
       <c r="C49" s="6"/>
@@ -5035,7 +5030,7 @@
       <c r="R49"/>
       <c r="S49"/>
     </row>
-    <row r="50" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" s="11" customFormat="1">
       <c r="A50"/>
       <c r="B50" s="23"/>
       <c r="C50" s="6"/>
@@ -5056,7 +5051,7 @@
       <c r="R50"/>
       <c r="S50"/>
     </row>
-    <row r="51" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" s="11" customFormat="1">
       <c r="A51"/>
       <c r="B51" s="23"/>
       <c r="C51" s="6"/>
@@ -5077,7 +5072,7 @@
       <c r="R51"/>
       <c r="S51"/>
     </row>
-    <row r="52" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" s="11" customFormat="1">
       <c r="A52"/>
       <c r="B52" s="23"/>
       <c r="C52" s="6"/>
@@ -5098,7 +5093,7 @@
       <c r="R52"/>
       <c r="S52"/>
     </row>
-    <row r="53" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" s="11" customFormat="1">
       <c r="A53"/>
       <c r="B53" s="23"/>
       <c r="C53" s="6"/>
@@ -5119,7 +5114,7 @@
       <c r="R53"/>
       <c r="S53"/>
     </row>
-    <row r="54" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" s="11" customFormat="1">
       <c r="A54"/>
       <c r="B54" s="23"/>
       <c r="C54" s="6"/>
@@ -5140,7 +5135,7 @@
       <c r="R54"/>
       <c r="S54"/>
     </row>
-    <row r="55" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" s="11" customFormat="1">
       <c r="A55"/>
       <c r="B55" s="23"/>
       <c r="C55" s="6"/>
@@ -5161,7 +5156,7 @@
       <c r="R55"/>
       <c r="S55"/>
     </row>
-    <row r="56" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" s="11" customFormat="1">
       <c r="A56"/>
       <c r="B56" s="23"/>
       <c r="C56" s="6"/>
@@ -5182,7 +5177,7 @@
       <c r="R56"/>
       <c r="S56"/>
     </row>
-    <row r="57" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" s="11" customFormat="1">
       <c r="A57"/>
       <c r="B57" s="23"/>
       <c r="C57" s="6"/>
@@ -5203,7 +5198,7 @@
       <c r="R57"/>
       <c r="S57"/>
     </row>
-    <row r="58" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" s="11" customFormat="1">
       <c r="A58"/>
       <c r="B58" s="23"/>
       <c r="C58" s="6"/>
@@ -5224,7 +5219,7 @@
       <c r="R58"/>
       <c r="S58"/>
     </row>
-    <row r="59" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" s="11" customFormat="1">
       <c r="A59"/>
       <c r="B59" s="23"/>
       <c r="C59" s="6"/>
@@ -5245,7 +5240,7 @@
       <c r="R59"/>
       <c r="S59"/>
     </row>
-    <row r="60" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" s="11" customFormat="1">
       <c r="A60"/>
       <c r="B60" s="23"/>
       <c r="C60" s="6"/>
@@ -5266,7 +5261,7 @@
       <c r="R60"/>
       <c r="S60"/>
     </row>
-    <row r="61" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" s="11" customFormat="1">
       <c r="A61"/>
       <c r="B61" s="23"/>
       <c r="C61" s="6"/>
@@ -5287,7 +5282,7 @@
       <c r="R61"/>
       <c r="S61"/>
     </row>
-    <row r="62" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" s="11" customFormat="1">
       <c r="A62"/>
       <c r="B62" s="23"/>
       <c r="C62" s="6"/>
@@ -5308,7 +5303,7 @@
       <c r="R62"/>
       <c r="S62"/>
     </row>
-    <row r="63" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" s="11" customFormat="1">
       <c r="A63"/>
       <c r="B63" s="23"/>
       <c r="C63" s="6"/>
@@ -5329,7 +5324,7 @@
       <c r="R63"/>
       <c r="S63"/>
     </row>
-    <row r="64" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" s="11" customFormat="1">
       <c r="A64"/>
       <c r="B64" s="23"/>
       <c r="C64" s="6"/>
@@ -5350,7 +5345,7 @@
       <c r="R64"/>
       <c r="S64"/>
     </row>
-    <row r="65" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" s="11" customFormat="1">
       <c r="A65"/>
       <c r="B65" s="23"/>
       <c r="C65" s="6"/>
@@ -5371,7 +5366,7 @@
       <c r="R65"/>
       <c r="S65"/>
     </row>
-    <row r="66" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" s="11" customFormat="1">
       <c r="A66"/>
       <c r="B66" s="23"/>
       <c r="C66" s="6"/>
@@ -5392,7 +5387,7 @@
       <c r="R66"/>
       <c r="S66"/>
     </row>
-    <row r="67" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" s="11" customFormat="1">
       <c r="A67"/>
       <c r="B67" s="23"/>
       <c r="C67" s="6"/>
@@ -5413,7 +5408,7 @@
       <c r="R67"/>
       <c r="S67"/>
     </row>
-    <row r="68" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" s="11" customFormat="1">
       <c r="A68"/>
       <c r="B68" s="23"/>
       <c r="C68" s="6"/>
@@ -5434,7 +5429,7 @@
       <c r="R68"/>
       <c r="S68"/>
     </row>
-    <row r="69" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" s="11" customFormat="1">
       <c r="A69"/>
       <c r="B69" s="23"/>
       <c r="C69" s="6"/>
@@ -5455,7 +5450,7 @@
       <c r="R69"/>
       <c r="S69"/>
     </row>
-    <row r="70" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" s="11" customFormat="1">
       <c r="A70"/>
       <c r="B70" s="23"/>
       <c r="C70" s="6"/>
@@ -5476,7 +5471,7 @@
       <c r="R70"/>
       <c r="S70"/>
     </row>
-    <row r="71" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" s="11" customFormat="1">
       <c r="A71"/>
       <c r="B71" s="23"/>
       <c r="C71" s="6"/>
@@ -5497,7 +5492,7 @@
       <c r="R71"/>
       <c r="S71"/>
     </row>
-    <row r="72" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" s="11" customFormat="1">
       <c r="A72"/>
       <c r="B72" s="23"/>
       <c r="C72" s="6"/>
@@ -5518,7 +5513,7 @@
       <c r="R72"/>
       <c r="S72"/>
     </row>
-    <row r="73" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" s="11" customFormat="1">
       <c r="A73"/>
       <c r="B73" s="23"/>
       <c r="C73" s="6"/>
@@ -5539,7 +5534,7 @@
       <c r="R73"/>
       <c r="S73"/>
     </row>
-    <row r="74" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" s="11" customFormat="1">
       <c r="A74"/>
       <c r="B74" s="23"/>
       <c r="C74" s="6"/>
@@ -5560,7 +5555,7 @@
       <c r="R74"/>
       <c r="S74"/>
     </row>
-    <row r="75" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" s="11" customFormat="1">
       <c r="A75"/>
       <c r="B75" s="23"/>
       <c r="C75" s="6"/>
@@ -5581,7 +5576,7 @@
       <c r="R75"/>
       <c r="S75"/>
     </row>
-    <row r="76" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" s="11" customFormat="1">
       <c r="A76"/>
       <c r="B76" s="23"/>
       <c r="C76" s="6"/>
@@ -5602,7 +5597,7 @@
       <c r="R76"/>
       <c r="S76"/>
     </row>
-    <row r="77" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" s="11" customFormat="1">
       <c r="A77"/>
       <c r="B77" s="23"/>
       <c r="C77" s="6"/>
@@ -5623,7 +5618,7 @@
       <c r="R77"/>
       <c r="S77"/>
     </row>
-    <row r="78" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" s="11" customFormat="1">
       <c r="A78"/>
       <c r="B78" s="23"/>
       <c r="C78" s="6"/>
@@ -5644,7 +5639,7 @@
       <c r="R78"/>
       <c r="S78"/>
     </row>
-    <row r="79" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" s="11" customFormat="1">
       <c r="A79"/>
       <c r="B79" s="23"/>
       <c r="C79" s="6"/>
@@ -5665,7 +5660,7 @@
       <c r="R79"/>
       <c r="S79"/>
     </row>
-    <row r="80" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" s="11" customFormat="1">
       <c r="A80"/>
       <c r="B80" s="23"/>
       <c r="C80" s="6"/>
@@ -5686,7 +5681,7 @@
       <c r="R80"/>
       <c r="S80"/>
     </row>
-    <row r="81" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" s="11" customFormat="1">
       <c r="A81"/>
       <c r="B81" s="23"/>
       <c r="C81" s="6"/>
@@ -5707,7 +5702,7 @@
       <c r="R81"/>
       <c r="S81"/>
     </row>
-    <row r="82" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" s="11" customFormat="1">
       <c r="A82"/>
       <c r="B82" s="23"/>
       <c r="C82" s="6"/>
@@ -5728,7 +5723,7 @@
       <c r="R82"/>
       <c r="S82"/>
     </row>
-    <row r="83" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" s="11" customFormat="1">
       <c r="A83"/>
       <c r="B83" s="23"/>
       <c r="C83" s="6"/>
@@ -5749,7 +5744,7 @@
       <c r="R83"/>
       <c r="S83"/>
     </row>
-    <row r="84" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" s="11" customFormat="1">
       <c r="A84"/>
       <c r="B84" s="23"/>
       <c r="C84" s="6"/>
@@ -5770,7 +5765,7 @@
       <c r="R84"/>
       <c r="S84"/>
     </row>
-    <row r="85" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" s="11" customFormat="1">
       <c r="A85"/>
       <c r="B85" s="23"/>
       <c r="C85" s="6"/>
@@ -5791,7 +5786,7 @@
       <c r="R85"/>
       <c r="S85"/>
     </row>
-    <row r="86" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" s="11" customFormat="1">
       <c r="A86"/>
       <c r="B86" s="23"/>
       <c r="C86" s="6"/>
@@ -5812,7 +5807,7 @@
       <c r="R86"/>
       <c r="S86"/>
     </row>
-    <row r="87" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" s="11" customFormat="1">
       <c r="A87"/>
       <c r="B87" s="23"/>
       <c r="C87" s="6"/>
@@ -5833,7 +5828,7 @@
       <c r="R87"/>
       <c r="S87"/>
     </row>
-    <row r="88" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" s="11" customFormat="1">
       <c r="A88"/>
       <c r="B88" s="23"/>
       <c r="C88" s="6"/>
@@ -5854,7 +5849,7 @@
       <c r="R88"/>
       <c r="S88"/>
     </row>
-    <row r="89" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" s="11" customFormat="1">
       <c r="A89"/>
       <c r="B89" s="23"/>
       <c r="C89" s="6"/>
@@ -5875,7 +5870,7 @@
       <c r="R89"/>
       <c r="S89"/>
     </row>
-    <row r="90" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" s="11" customFormat="1">
       <c r="A90"/>
       <c r="B90" s="23"/>
       <c r="C90" s="6"/>
@@ -5896,7 +5891,7 @@
       <c r="R90"/>
       <c r="S90"/>
     </row>
-    <row r="91" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" s="11" customFormat="1">
       <c r="A91"/>
       <c r="B91" s="23"/>
       <c r="C91" s="6"/>
@@ -5917,7 +5912,7 @@
       <c r="R91"/>
       <c r="S91"/>
     </row>
-    <row r="92" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" s="11" customFormat="1">
       <c r="A92"/>
       <c r="B92" s="23"/>
       <c r="C92" s="6"/>
@@ -5938,7 +5933,7 @@
       <c r="R92"/>
       <c r="S92"/>
     </row>
-    <row r="93" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" s="11" customFormat="1">
       <c r="A93"/>
       <c r="B93" s="23"/>
       <c r="C93" s="6"/>
@@ -5959,7 +5954,7 @@
       <c r="R93"/>
       <c r="S93"/>
     </row>
-    <row r="94" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" s="11" customFormat="1">
       <c r="A94"/>
       <c r="B94" s="23"/>
       <c r="C94" s="6"/>
@@ -5980,7 +5975,7 @@
       <c r="R94"/>
       <c r="S94"/>
     </row>
-    <row r="95" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" s="11" customFormat="1">
       <c r="A95"/>
       <c r="B95" s="23"/>
       <c r="C95" s="6"/>
@@ -6001,7 +5996,7 @@
       <c r="R95"/>
       <c r="S95"/>
     </row>
-    <row r="96" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" s="11" customFormat="1">
       <c r="A96"/>
       <c r="B96" s="23"/>
       <c r="C96" s="6"/>
@@ -6022,7 +6017,7 @@
       <c r="R96"/>
       <c r="S96"/>
     </row>
-    <row r="97" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" s="11" customFormat="1">
       <c r="A97"/>
       <c r="B97" s="23"/>
       <c r="C97" s="6"/>
@@ -6043,7 +6038,7 @@
       <c r="R97"/>
       <c r="S97"/>
     </row>
-    <row r="98" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" s="11" customFormat="1">
       <c r="A98"/>
       <c r="B98" s="23"/>
       <c r="C98" s="6"/>
@@ -6064,7 +6059,7 @@
       <c r="R98"/>
       <c r="S98"/>
     </row>
-    <row r="99" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" s="11" customFormat="1">
       <c r="A99"/>
       <c r="B99" s="23"/>
       <c r="C99" s="6"/>
@@ -6085,7 +6080,7 @@
       <c r="R99"/>
       <c r="S99"/>
     </row>
-    <row r="100" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" s="11" customFormat="1">
       <c r="A100"/>
       <c r="B100" s="23"/>
       <c r="C100" s="6"/>
@@ -6106,7 +6101,7 @@
       <c r="R100"/>
       <c r="S100"/>
     </row>
-    <row r="101" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" s="11" customFormat="1">
       <c r="A101"/>
       <c r="B101" s="23"/>
       <c r="C101" s="6"/>
@@ -6127,7 +6122,7 @@
       <c r="R101"/>
       <c r="S101"/>
     </row>
-    <row r="102" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" s="11" customFormat="1">
       <c r="A102"/>
       <c r="B102" s="23"/>
       <c r="C102" s="6"/>
@@ -6148,7 +6143,7 @@
       <c r="R102"/>
       <c r="S102"/>
     </row>
-    <row r="103" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" s="11" customFormat="1">
       <c r="A103"/>
       <c r="B103" s="23"/>
       <c r="C103" s="6"/>
@@ -6169,7 +6164,7 @@
       <c r="R103"/>
       <c r="S103"/>
     </row>
-    <row r="104" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" s="11" customFormat="1">
       <c r="A104"/>
       <c r="B104" s="23"/>
       <c r="C104" s="6"/>
@@ -6190,7 +6185,7 @@
       <c r="R104"/>
       <c r="S104"/>
     </row>
-    <row r="105" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" s="11" customFormat="1">
       <c r="A105"/>
       <c r="B105" s="23"/>
       <c r="C105" s="6"/>
@@ -6211,7 +6206,7 @@
       <c r="R105"/>
       <c r="S105"/>
     </row>
-    <row r="106" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" s="11" customFormat="1">
       <c r="A106"/>
       <c r="B106" s="23"/>
       <c r="C106" s="6"/>
@@ -6232,7 +6227,7 @@
       <c r="R106"/>
       <c r="S106"/>
     </row>
-    <row r="107" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" s="11" customFormat="1">
       <c r="A107"/>
       <c r="B107" s="23"/>
       <c r="C107" s="6"/>
@@ -6253,7 +6248,7 @@
       <c r="R107"/>
       <c r="S107"/>
     </row>
-    <row r="108" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" s="11" customFormat="1">
       <c r="A108"/>
       <c r="B108" s="23"/>
       <c r="C108" s="6"/>
@@ -6274,7 +6269,7 @@
       <c r="R108"/>
       <c r="S108"/>
     </row>
-    <row r="109" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" s="11" customFormat="1">
       <c r="A109"/>
       <c r="B109" s="23"/>
       <c r="C109" s="6"/>
@@ -6295,7 +6290,7 @@
       <c r="R109"/>
       <c r="S109"/>
     </row>
-    <row r="110" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" s="11" customFormat="1">
       <c r="A110"/>
       <c r="B110" s="23"/>
       <c r="C110" s="6"/>
@@ -6316,7 +6311,7 @@
       <c r="R110"/>
       <c r="S110"/>
     </row>
-    <row r="111" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" s="11" customFormat="1">
       <c r="A111"/>
       <c r="B111" s="23"/>
       <c r="C111" s="6"/>
@@ -6337,7 +6332,7 @@
       <c r="R111"/>
       <c r="S111"/>
     </row>
-    <row r="112" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" s="11" customFormat="1">
       <c r="A112"/>
       <c r="B112" s="23"/>
       <c r="C112" s="6"/>
@@ -6358,7 +6353,7 @@
       <c r="R112"/>
       <c r="S112"/>
     </row>
-    <row r="113" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" s="11" customFormat="1">
       <c r="A113"/>
       <c r="B113" s="23"/>
       <c r="C113" s="6"/>
@@ -6379,7 +6374,7 @@
       <c r="R113"/>
       <c r="S113"/>
     </row>
-    <row r="114" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" s="11" customFormat="1">
       <c r="A114"/>
       <c r="B114" s="23"/>
       <c r="C114" s="6"/>
@@ -6400,7 +6395,7 @@
       <c r="R114"/>
       <c r="S114"/>
     </row>
-    <row r="115" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" s="11" customFormat="1">
       <c r="A115"/>
       <c r="B115" s="23"/>
       <c r="C115" s="6"/>
@@ -6421,7 +6416,7 @@
       <c r="R115"/>
       <c r="S115"/>
     </row>
-    <row r="116" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" s="11" customFormat="1">
       <c r="A116"/>
       <c r="B116" s="23"/>
       <c r="C116" s="6"/>
@@ -6442,7 +6437,7 @@
       <c r="R116"/>
       <c r="S116"/>
     </row>
-    <row r="117" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" s="11" customFormat="1">
       <c r="A117"/>
       <c r="B117" s="23"/>
       <c r="C117" s="6"/>
@@ -6463,7 +6458,7 @@
       <c r="R117"/>
       <c r="S117"/>
     </row>
-    <row r="118" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" s="11" customFormat="1">
       <c r="A118"/>
       <c r="B118" s="23"/>
       <c r="C118" s="6"/>
@@ -6507,32 +6502,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B55" sqref="B55"/>
       <selection pane="topRight" activeCell="B55" sqref="B55"/>
       <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15:C16"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="2" width="83.375" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="83.33203125" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="6" customWidth="1"/>
     <col min="4" max="4" width="11" style="6"/>
-    <col min="5" max="5" width="44.375" customWidth="1"/>
-    <col min="6" max="6" width="27.875" customWidth="1"/>
-    <col min="7" max="7" width="24.375" customWidth="1"/>
-    <col min="8" max="8" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" s="32" t="s">
         <v>5</v>
       </c>
@@ -6545,7 +6540,7 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="30">
       <c r="B2" s="36" t="s">
         <v>8</v>
       </c>
@@ -6568,7 +6563,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="43" t="s">
         <v>128</v>
       </c>
@@ -6579,7 +6574,7 @@
       <c r="G3" s="48"/>
       <c r="H3" s="48"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="24"/>
       <c r="E4" s="55"/>
@@ -6587,7 +6582,7 @@
       <c r="G4" s="48"/>
       <c r="H4" s="48"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="71" t="s">
         <v>1</v>
       </c>
@@ -6609,7 +6604,7 @@
         <v>Identify different social media channels that are both being used in your organisation and not. Mention has to be up to date with actual implementation.</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="71"/>
       <c r="B6" s="25" t="s">
         <v>45</v>
@@ -6629,7 +6624,7 @@
         <v>Identify and differentiate the usage of existing social media channels such as how they target different audience groups and serve up different content.</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="71"/>
       <c r="B7" s="26" t="s">
         <v>46</v>
@@ -6649,7 +6644,7 @@
         <v>Acknowledge other social media channels other than Facebook, Twitter and YouTube. Mention could include the choice of the organisation to not use other social media channels.</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="71"/>
       <c r="B8" s="16" t="s">
         <v>14</v>
@@ -6676,10 +6671,10 @@
         <v>Identify different social media channels that are both being used in your organisation and not. Mention has to be up to date with actual implementation.Identify and differentiate the usage of existing social media channels such as how they target different audience groups and serve up different content.Acknowledge other social media channels other than Facebook, Twitter and YouTube. Mention could include the choice of the organisation to not use other social media channels.</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="8"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="70" t="s">
         <v>3</v>
       </c>
@@ -6701,7 +6696,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="70"/>
       <c r="B11" s="27" t="s">
         <v>28</v>
@@ -6721,7 +6716,7 @@
         <v>Determine who is tasked with monitoring and responding to social media channels and their escalation paths.</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="70"/>
       <c r="B12" s="27" t="s">
         <v>48</v>
@@ -6741,7 +6736,7 @@
         <v>Define guidelines for the tone of voice to adopt on your social media channels. Base this on your organisation’s brand guidelines, but take into account potential differences in the audiences of your social media channels.</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="70"/>
       <c r="B13" s="20" t="s">
         <v>16</v>
@@ -6768,8 +6763,8 @@
         <v>Determine who is tasked with monitoring and responding to social media channels and their escalation paths.Define guidelines for the tone of voice to adopt on your social media channels. Base this on your organisation’s brand guidelines, but take into account potential differences in the audiences of your social media channels.</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1"/>
+    <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="70" t="s">
         <v>30</v>
       </c>
@@ -6791,7 +6786,7 @@
         <v>Define a organisation-wide policy for responding on social channels. This could include response time, personnel tasked to respond and response etiquette. Even if you decide not to respond, you should declare why in your social media strategy.</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="70"/>
       <c r="B16" s="27" t="s">
         <v>26</v>
@@ -6811,7 +6806,7 @@
         <v>Define how staff who are tasked with community management should respond to complaints on social media channels. This could include a workflow or approval process wherein the complaint and response gets approved by certain personnel before being published.</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="15" customHeight="1">
       <c r="A17" s="70"/>
       <c r="B17" s="20" t="s">
         <v>62</v>
@@ -6838,10 +6833,10 @@
         <v>Define a organisation-wide policy for responding on social channels. This could include response time, personnel tasked to respond and response etiquette. Even if you decide not to respond, you should declare why in your social media strategy.Define how staff who are tasked with community management should respond to complaints on social media channels. This could include a workflow or approval process wherein the complaint and response gets approved by certain personnel before being published.</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="15" customHeight="1"/>
+    <row r="19" spans="1:20" ht="15" customHeight="1"/>
+    <row r="20" spans="1:20" ht="15" customHeight="1"/>
+    <row r="21" spans="1:20" s="11" customFormat="1">
       <c r="A21"/>
       <c r="B21" s="23"/>
       <c r="C21" s="6"/>
@@ -6863,7 +6858,7 @@
       <c r="S21"/>
       <c r="T21"/>
     </row>
-    <row r="22" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" s="11" customFormat="1">
       <c r="A22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="6"/>
@@ -6885,7 +6880,7 @@
       <c r="S22"/>
       <c r="T22"/>
     </row>
-    <row r="23" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" s="11" customFormat="1">
       <c r="A23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="6"/>
@@ -6907,7 +6902,7 @@
       <c r="S23"/>
       <c r="T23"/>
     </row>
-    <row r="24" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" s="11" customFormat="1">
       <c r="A24"/>
       <c r="B24" s="23"/>
       <c r="C24" s="6"/>
@@ -6929,7 +6924,7 @@
       <c r="S24"/>
       <c r="T24"/>
     </row>
-    <row r="25" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="11" customFormat="1">
       <c r="A25"/>
       <c r="B25" s="23"/>
       <c r="C25" s="6"/>
@@ -6951,7 +6946,7 @@
       <c r="S25"/>
       <c r="T25"/>
     </row>
-    <row r="26" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="11" customFormat="1">
       <c r="A26"/>
       <c r="B26" s="23"/>
       <c r="C26" s="6"/>
@@ -6973,7 +6968,7 @@
       <c r="S26"/>
       <c r="T26"/>
     </row>
-    <row r="27" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="11" customFormat="1">
       <c r="A27"/>
       <c r="B27" s="23"/>
       <c r="C27" s="6"/>
@@ -6995,7 +6990,7 @@
       <c r="S27"/>
       <c r="T27"/>
     </row>
-    <row r="28" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" s="11" customFormat="1">
       <c r="A28"/>
       <c r="B28" s="23"/>
       <c r="C28" s="6"/>
@@ -7017,7 +7012,7 @@
       <c r="S28"/>
       <c r="T28"/>
     </row>
-    <row r="29" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" s="11" customFormat="1">
       <c r="A29"/>
       <c r="B29" s="23"/>
       <c r="C29" s="6"/>
@@ -7039,7 +7034,7 @@
       <c r="S29"/>
       <c r="T29"/>
     </row>
-    <row r="30" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" s="11" customFormat="1">
       <c r="A30"/>
       <c r="B30" s="23"/>
       <c r="C30" s="6"/>
@@ -7061,7 +7056,7 @@
       <c r="S30"/>
       <c r="T30"/>
     </row>
-    <row r="31" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" s="11" customFormat="1">
       <c r="A31"/>
       <c r="B31" s="23"/>
       <c r="C31" s="6"/>
@@ -7083,7 +7078,7 @@
       <c r="S31"/>
       <c r="T31"/>
     </row>
-    <row r="32" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" s="11" customFormat="1">
       <c r="A32"/>
       <c r="B32" s="23"/>
       <c r="C32" s="6"/>
@@ -7105,7 +7100,7 @@
       <c r="S32"/>
       <c r="T32"/>
     </row>
-    <row r="33" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" s="11" customFormat="1">
       <c r="A33"/>
       <c r="B33" s="23"/>
       <c r="C33" s="6"/>
@@ -7127,7 +7122,7 @@
       <c r="S33"/>
       <c r="T33"/>
     </row>
-    <row r="34" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" s="11" customFormat="1">
       <c r="A34"/>
       <c r="B34" s="23"/>
       <c r="C34" s="6"/>
@@ -7149,7 +7144,7 @@
       <c r="S34"/>
       <c r="T34"/>
     </row>
-    <row r="35" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" s="11" customFormat="1">
       <c r="A35"/>
       <c r="B35" s="23"/>
       <c r="C35" s="6"/>
@@ -7171,7 +7166,7 @@
       <c r="S35"/>
       <c r="T35"/>
     </row>
-    <row r="36" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" s="11" customFormat="1">
       <c r="A36"/>
       <c r="B36" s="23"/>
       <c r="C36" s="6"/>
@@ -7193,7 +7188,7 @@
       <c r="S36"/>
       <c r="T36"/>
     </row>
-    <row r="37" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" s="11" customFormat="1">
       <c r="A37"/>
       <c r="B37" s="23"/>
       <c r="C37" s="6"/>
@@ -7215,7 +7210,7 @@
       <c r="S37"/>
       <c r="T37"/>
     </row>
-    <row r="38" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" s="11" customFormat="1">
       <c r="A38"/>
       <c r="B38" s="23"/>
       <c r="C38" s="6"/>
@@ -7237,7 +7232,7 @@
       <c r="S38"/>
       <c r="T38"/>
     </row>
-    <row r="39" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" s="11" customFormat="1">
       <c r="A39"/>
       <c r="B39" s="23"/>
       <c r="C39" s="6"/>
@@ -7259,7 +7254,7 @@
       <c r="S39"/>
       <c r="T39"/>
     </row>
-    <row r="40" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" s="11" customFormat="1">
       <c r="A40"/>
       <c r="B40" s="23"/>
       <c r="C40" s="6"/>
@@ -7281,7 +7276,7 @@
       <c r="S40"/>
       <c r="T40"/>
     </row>
-    <row r="41" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" s="11" customFormat="1">
       <c r="A41"/>
       <c r="B41" s="23"/>
       <c r="C41" s="6"/>
@@ -7303,7 +7298,7 @@
       <c r="S41"/>
       <c r="T41"/>
     </row>
-    <row r="42" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" s="11" customFormat="1">
       <c r="A42"/>
       <c r="B42" s="23"/>
       <c r="C42" s="6"/>
@@ -7325,7 +7320,7 @@
       <c r="S42"/>
       <c r="T42"/>
     </row>
-    <row r="43" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" s="11" customFormat="1">
       <c r="A43"/>
       <c r="B43" s="23"/>
       <c r="C43" s="6"/>
@@ -7347,7 +7342,7 @@
       <c r="S43"/>
       <c r="T43"/>
     </row>
-    <row r="44" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" s="11" customFormat="1">
       <c r="A44"/>
       <c r="B44" s="23"/>
       <c r="C44" s="6"/>
@@ -7369,7 +7364,7 @@
       <c r="S44"/>
       <c r="T44"/>
     </row>
-    <row r="45" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" s="11" customFormat="1">
       <c r="A45"/>
       <c r="B45" s="23"/>
       <c r="C45" s="6"/>
@@ -7391,7 +7386,7 @@
       <c r="S45"/>
       <c r="T45"/>
     </row>
-    <row r="46" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" s="11" customFormat="1">
       <c r="A46"/>
       <c r="B46" s="23"/>
       <c r="C46" s="6"/>
@@ -7413,7 +7408,7 @@
       <c r="S46"/>
       <c r="T46"/>
     </row>
-    <row r="47" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" s="11" customFormat="1">
       <c r="A47"/>
       <c r="B47" s="23"/>
       <c r="C47" s="6"/>
@@ -7435,7 +7430,7 @@
       <c r="S47"/>
       <c r="T47"/>
     </row>
-    <row r="48" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" s="11" customFormat="1">
       <c r="A48"/>
       <c r="B48" s="23"/>
       <c r="C48" s="6"/>
@@ -7457,7 +7452,7 @@
       <c r="S48"/>
       <c r="T48"/>
     </row>
-    <row r="49" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" s="11" customFormat="1">
       <c r="A49"/>
       <c r="B49" s="23"/>
       <c r="C49" s="6"/>
@@ -7479,7 +7474,7 @@
       <c r="S49"/>
       <c r="T49"/>
     </row>
-    <row r="50" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" s="11" customFormat="1">
       <c r="A50"/>
       <c r="B50" s="23"/>
       <c r="C50" s="6"/>
@@ -7501,7 +7496,7 @@
       <c r="S50"/>
       <c r="T50"/>
     </row>
-    <row r="51" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" s="11" customFormat="1">
       <c r="A51"/>
       <c r="B51" s="23"/>
       <c r="C51" s="6"/>
@@ -7523,7 +7518,7 @@
       <c r="S51"/>
       <c r="T51"/>
     </row>
-    <row r="52" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" s="11" customFormat="1">
       <c r="A52"/>
       <c r="B52" s="23"/>
       <c r="C52" s="6"/>
@@ -7545,7 +7540,7 @@
       <c r="S52"/>
       <c r="T52"/>
     </row>
-    <row r="53" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" s="11" customFormat="1">
       <c r="A53"/>
       <c r="B53" s="23"/>
       <c r="C53" s="6"/>
@@ -7567,7 +7562,7 @@
       <c r="S53"/>
       <c r="T53"/>
     </row>
-    <row r="54" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" s="11" customFormat="1">
       <c r="A54"/>
       <c r="B54" s="23"/>
       <c r="C54" s="6"/>
@@ -7589,7 +7584,7 @@
       <c r="S54"/>
       <c r="T54"/>
     </row>
-    <row r="55" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" s="11" customFormat="1">
       <c r="A55"/>
       <c r="B55" s="23"/>
       <c r="C55" s="6"/>
@@ -7611,7 +7606,7 @@
       <c r="S55"/>
       <c r="T55"/>
     </row>
-    <row r="56" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" s="11" customFormat="1">
       <c r="A56"/>
       <c r="B56" s="23"/>
       <c r="C56" s="6"/>
@@ -7633,7 +7628,7 @@
       <c r="S56"/>
       <c r="T56"/>
     </row>
-    <row r="57" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" s="11" customFormat="1">
       <c r="A57"/>
       <c r="B57" s="23"/>
       <c r="C57" s="6"/>
@@ -7655,7 +7650,7 @@
       <c r="S57"/>
       <c r="T57"/>
     </row>
-    <row r="58" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" s="11" customFormat="1">
       <c r="A58"/>
       <c r="B58" s="23"/>
       <c r="C58" s="6"/>
@@ -7677,7 +7672,7 @@
       <c r="S58"/>
       <c r="T58"/>
     </row>
-    <row r="59" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" s="11" customFormat="1">
       <c r="A59"/>
       <c r="B59" s="23"/>
       <c r="C59" s="6"/>
@@ -7699,7 +7694,7 @@
       <c r="S59"/>
       <c r="T59"/>
     </row>
-    <row r="60" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" s="11" customFormat="1">
       <c r="A60"/>
       <c r="B60" s="23"/>
       <c r="C60" s="6"/>
@@ -7721,7 +7716,7 @@
       <c r="S60"/>
       <c r="T60"/>
     </row>
-    <row r="61" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" s="11" customFormat="1">
       <c r="A61"/>
       <c r="B61" s="23"/>
       <c r="C61" s="6"/>
@@ -7743,7 +7738,7 @@
       <c r="S61"/>
       <c r="T61"/>
     </row>
-    <row r="62" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" s="11" customFormat="1">
       <c r="A62"/>
       <c r="B62" s="23"/>
       <c r="C62" s="6"/>
@@ -7765,7 +7760,7 @@
       <c r="S62"/>
       <c r="T62"/>
     </row>
-    <row r="63" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" s="11" customFormat="1">
       <c r="A63"/>
       <c r="B63" s="23"/>
       <c r="C63" s="6"/>
@@ -7787,7 +7782,7 @@
       <c r="S63"/>
       <c r="T63"/>
     </row>
-    <row r="64" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" s="11" customFormat="1">
       <c r="A64"/>
       <c r="B64" s="23"/>
       <c r="C64" s="6"/>
@@ -7809,7 +7804,7 @@
       <c r="S64"/>
       <c r="T64"/>
     </row>
-    <row r="65" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" s="11" customFormat="1">
       <c r="A65"/>
       <c r="B65" s="23"/>
       <c r="C65" s="6"/>
@@ -7831,7 +7826,7 @@
       <c r="S65"/>
       <c r="T65"/>
     </row>
-    <row r="66" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" s="11" customFormat="1">
       <c r="A66"/>
       <c r="B66" s="23"/>
       <c r="C66" s="6"/>
@@ -7853,7 +7848,7 @@
       <c r="S66"/>
       <c r="T66"/>
     </row>
-    <row r="67" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" s="11" customFormat="1">
       <c r="A67"/>
       <c r="B67" s="23"/>
       <c r="C67" s="6"/>
@@ -7875,7 +7870,7 @@
       <c r="S67"/>
       <c r="T67"/>
     </row>
-    <row r="68" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" s="11" customFormat="1">
       <c r="A68"/>
       <c r="B68" s="23"/>
       <c r="C68" s="6"/>
@@ -7897,7 +7892,7 @@
       <c r="S68"/>
       <c r="T68"/>
     </row>
-    <row r="69" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" s="11" customFormat="1">
       <c r="A69"/>
       <c r="B69" s="23"/>
       <c r="C69" s="6"/>
@@ -7919,7 +7914,7 @@
       <c r="S69"/>
       <c r="T69"/>
     </row>
-    <row r="70" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" s="11" customFormat="1">
       <c r="A70"/>
       <c r="B70" s="23"/>
       <c r="C70" s="6"/>
@@ -7941,7 +7936,7 @@
       <c r="S70"/>
       <c r="T70"/>
     </row>
-    <row r="71" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" s="11" customFormat="1">
       <c r="A71"/>
       <c r="B71" s="23"/>
       <c r="C71" s="6"/>
@@ -7963,7 +7958,7 @@
       <c r="S71"/>
       <c r="T71"/>
     </row>
-    <row r="72" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" s="11" customFormat="1">
       <c r="A72"/>
       <c r="B72" s="23"/>
       <c r="C72" s="6"/>
@@ -7985,7 +7980,7 @@
       <c r="S72"/>
       <c r="T72"/>
     </row>
-    <row r="73" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" s="11" customFormat="1">
       <c r="A73"/>
       <c r="B73" s="23"/>
       <c r="C73" s="6"/>
@@ -8007,7 +8002,7 @@
       <c r="S73"/>
       <c r="T73"/>
     </row>
-    <row r="74" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" s="11" customFormat="1">
       <c r="A74"/>
       <c r="B74" s="23"/>
       <c r="C74" s="6"/>
@@ -8029,7 +8024,7 @@
       <c r="S74"/>
       <c r="T74"/>
     </row>
-    <row r="75" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" s="11" customFormat="1">
       <c r="A75"/>
       <c r="B75" s="23"/>
       <c r="C75" s="6"/>
@@ -8051,7 +8046,7 @@
       <c r="S75"/>
       <c r="T75"/>
     </row>
-    <row r="76" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" s="11" customFormat="1">
       <c r="A76"/>
       <c r="B76" s="23"/>
       <c r="C76" s="6"/>
@@ -8073,7 +8068,7 @@
       <c r="S76"/>
       <c r="T76"/>
     </row>
-    <row r="77" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" s="11" customFormat="1">
       <c r="A77"/>
       <c r="B77" s="23"/>
       <c r="C77" s="6"/>
@@ -8095,7 +8090,7 @@
       <c r="S77"/>
       <c r="T77"/>
     </row>
-    <row r="78" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" s="11" customFormat="1">
       <c r="A78"/>
       <c r="B78" s="23"/>
       <c r="C78" s="6"/>
@@ -8117,7 +8112,7 @@
       <c r="S78"/>
       <c r="T78"/>
     </row>
-    <row r="79" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" s="11" customFormat="1">
       <c r="A79"/>
       <c r="B79" s="23"/>
       <c r="C79" s="6"/>
@@ -8139,7 +8134,7 @@
       <c r="S79"/>
       <c r="T79"/>
     </row>
-    <row r="80" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" s="11" customFormat="1">
       <c r="A80"/>
       <c r="B80" s="23"/>
       <c r="C80" s="6"/>
@@ -8161,7 +8156,7 @@
       <c r="S80"/>
       <c r="T80"/>
     </row>
-    <row r="81" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" s="11" customFormat="1">
       <c r="A81"/>
       <c r="B81" s="23"/>
       <c r="C81" s="6"/>
@@ -8183,7 +8178,7 @@
       <c r="S81"/>
       <c r="T81"/>
     </row>
-    <row r="82" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" s="11" customFormat="1">
       <c r="A82"/>
       <c r="B82" s="23"/>
       <c r="C82" s="6"/>
@@ -8205,7 +8200,7 @@
       <c r="S82"/>
       <c r="T82"/>
     </row>
-    <row r="83" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" s="11" customFormat="1">
       <c r="A83"/>
       <c r="B83" s="23"/>
       <c r="C83" s="6"/>
@@ -8227,7 +8222,7 @@
       <c r="S83"/>
       <c r="T83"/>
     </row>
-    <row r="84" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" s="11" customFormat="1">
       <c r="A84"/>
       <c r="B84" s="23"/>
       <c r="C84" s="6"/>
@@ -8249,7 +8244,7 @@
       <c r="S84"/>
       <c r="T84"/>
     </row>
-    <row r="85" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" s="11" customFormat="1">
       <c r="A85"/>
       <c r="B85" s="23"/>
       <c r="C85" s="6"/>
@@ -8271,7 +8266,7 @@
       <c r="S85"/>
       <c r="T85"/>
     </row>
-    <row r="86" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" s="11" customFormat="1">
       <c r="A86"/>
       <c r="B86" s="23"/>
       <c r="C86" s="6"/>
@@ -8293,7 +8288,7 @@
       <c r="S86"/>
       <c r="T86"/>
     </row>
-    <row r="87" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" s="11" customFormat="1">
       <c r="A87"/>
       <c r="B87" s="23"/>
       <c r="C87" s="6"/>
@@ -8315,7 +8310,7 @@
       <c r="S87"/>
       <c r="T87"/>
     </row>
-    <row r="88" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" s="11" customFormat="1">
       <c r="A88"/>
       <c r="B88" s="23"/>
       <c r="C88" s="6"/>
@@ -8337,7 +8332,7 @@
       <c r="S88"/>
       <c r="T88"/>
     </row>
-    <row r="89" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" s="11" customFormat="1">
       <c r="A89"/>
       <c r="B89" s="23"/>
       <c r="C89" s="6"/>
@@ -8359,7 +8354,7 @@
       <c r="S89"/>
       <c r="T89"/>
     </row>
-    <row r="90" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" s="11" customFormat="1">
       <c r="A90"/>
       <c r="B90" s="23"/>
       <c r="C90" s="6"/>
@@ -8381,7 +8376,7 @@
       <c r="S90"/>
       <c r="T90"/>
     </row>
-    <row r="91" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" s="11" customFormat="1">
       <c r="A91"/>
       <c r="B91" s="23"/>
       <c r="C91" s="6"/>
@@ -8403,7 +8398,7 @@
       <c r="S91"/>
       <c r="T91"/>
     </row>
-    <row r="92" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" s="11" customFormat="1">
       <c r="A92"/>
       <c r="B92" s="23"/>
       <c r="C92" s="6"/>
@@ -8425,7 +8420,7 @@
       <c r="S92"/>
       <c r="T92"/>
     </row>
-    <row r="93" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" s="11" customFormat="1">
       <c r="A93"/>
       <c r="B93" s="23"/>
       <c r="C93" s="6"/>
@@ -8447,7 +8442,7 @@
       <c r="S93"/>
       <c r="T93"/>
     </row>
-    <row r="94" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" s="11" customFormat="1">
       <c r="A94"/>
       <c r="B94" s="23"/>
       <c r="C94" s="6"/>
@@ -8469,7 +8464,7 @@
       <c r="S94"/>
       <c r="T94"/>
     </row>
-    <row r="95" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" s="11" customFormat="1">
       <c r="A95"/>
       <c r="B95" s="23"/>
       <c r="C95" s="6"/>
@@ -8491,7 +8486,7 @@
       <c r="S95"/>
       <c r="T95"/>
     </row>
-    <row r="96" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" s="11" customFormat="1">
       <c r="A96"/>
       <c r="B96" s="23"/>
       <c r="C96" s="6"/>
@@ -8513,7 +8508,7 @@
       <c r="S96"/>
       <c r="T96"/>
     </row>
-    <row r="97" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" s="11" customFormat="1">
       <c r="A97"/>
       <c r="B97" s="23"/>
       <c r="C97" s="6"/>
@@ -8535,7 +8530,7 @@
       <c r="S97"/>
       <c r="T97"/>
     </row>
-    <row r="98" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" s="11" customFormat="1">
       <c r="A98"/>
       <c r="B98" s="23"/>
       <c r="C98" s="6"/>
@@ -8557,7 +8552,7 @@
       <c r="S98"/>
       <c r="T98"/>
     </row>
-    <row r="99" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" s="11" customFormat="1">
       <c r="A99"/>
       <c r="B99" s="23"/>
       <c r="C99" s="6"/>
@@ -8579,7 +8574,7 @@
       <c r="S99"/>
       <c r="T99"/>
     </row>
-    <row r="100" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" s="11" customFormat="1">
       <c r="A100"/>
       <c r="B100" s="23"/>
       <c r="C100" s="6"/>
@@ -8601,7 +8596,7 @@
       <c r="S100"/>
       <c r="T100"/>
     </row>
-    <row r="101" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" s="11" customFormat="1">
       <c r="A101"/>
       <c r="B101" s="23"/>
       <c r="C101" s="6"/>
@@ -8623,7 +8618,7 @@
       <c r="S101"/>
       <c r="T101"/>
     </row>
-    <row r="102" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" s="11" customFormat="1">
       <c r="A102"/>
       <c r="B102" s="23"/>
       <c r="C102" s="6"/>
@@ -8645,7 +8640,7 @@
       <c r="S102"/>
       <c r="T102"/>
     </row>
-    <row r="103" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" s="11" customFormat="1">
       <c r="A103"/>
       <c r="B103" s="23"/>
       <c r="C103" s="6"/>
@@ -8667,7 +8662,7 @@
       <c r="S103"/>
       <c r="T103"/>
     </row>
-    <row r="104" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" s="11" customFormat="1">
       <c r="A104"/>
       <c r="B104" s="23"/>
       <c r="C104" s="6"/>
@@ -8689,7 +8684,7 @@
       <c r="S104"/>
       <c r="T104"/>
     </row>
-    <row r="105" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" s="11" customFormat="1">
       <c r="A105"/>
       <c r="B105" s="23"/>
       <c r="C105" s="6"/>
@@ -8711,7 +8706,7 @@
       <c r="S105"/>
       <c r="T105"/>
     </row>
-    <row r="106" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" s="11" customFormat="1">
       <c r="A106"/>
       <c r="B106" s="23"/>
       <c r="C106" s="6"/>
@@ -8733,7 +8728,7 @@
       <c r="S106"/>
       <c r="T106"/>
     </row>
-    <row r="107" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" s="11" customFormat="1">
       <c r="A107"/>
       <c r="B107" s="23"/>
       <c r="C107" s="6"/>
@@ -8755,7 +8750,7 @@
       <c r="S107"/>
       <c r="T107"/>
     </row>
-    <row r="108" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" s="11" customFormat="1">
       <c r="A108"/>
       <c r="B108" s="23"/>
       <c r="C108" s="6"/>
@@ -8777,7 +8772,7 @@
       <c r="S108"/>
       <c r="T108"/>
     </row>
-    <row r="109" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" s="11" customFormat="1">
       <c r="A109"/>
       <c r="B109" s="23"/>
       <c r="C109" s="6"/>
@@ -8799,7 +8794,7 @@
       <c r="S109"/>
       <c r="T109"/>
     </row>
-    <row r="110" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" s="11" customFormat="1">
       <c r="A110"/>
       <c r="B110" s="23"/>
       <c r="C110" s="6"/>
@@ -8821,7 +8816,7 @@
       <c r="S110"/>
       <c r="T110"/>
     </row>
-    <row r="111" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" s="11" customFormat="1">
       <c r="A111"/>
       <c r="B111" s="23"/>
       <c r="C111" s="6"/>
@@ -8843,7 +8838,7 @@
       <c r="S111"/>
       <c r="T111"/>
     </row>
-    <row r="112" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" s="11" customFormat="1">
       <c r="A112"/>
       <c r="B112" s="23"/>
       <c r="C112" s="6"/>
@@ -8865,7 +8860,7 @@
       <c r="S112"/>
       <c r="T112"/>
     </row>
-    <row r="113" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" s="11" customFormat="1">
       <c r="A113"/>
       <c r="B113" s="23"/>
       <c r="C113" s="6"/>
@@ -8894,11 +8889,8 @@
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A15:A17"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7 C10:C12 C16">
-      <formula1>$G$5:$G$6</formula1>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15">
+  <dataValidations count="1">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C5:C7 C10 C11 C12 C15 C16">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -8915,7 +8907,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:T118"/>
@@ -8925,21 +8917,21 @@
       <selection activeCell="B55" sqref="B55"/>
       <selection pane="topRight" activeCell="B55" sqref="B55"/>
       <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="2" width="82.625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="82.6640625" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" style="6"/>
-    <col min="5" max="5" width="44.375" customWidth="1"/>
-    <col min="6" max="6" width="27.875" customWidth="1"/>
-    <col min="7" max="7" width="24.375" customWidth="1"/>
-    <col min="8" max="8" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" s="32" t="s">
         <v>6</v>
       </c>
@@ -8952,7 +8944,7 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="30">
       <c r="B2" s="36" t="s">
         <v>8</v>
       </c>
@@ -8975,7 +8967,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="3" customFormat="1">
       <c r="A3" s="43" t="s">
         <v>145</v>
       </c>
@@ -8986,7 +8978,7 @@
       <c r="G3" s="48"/>
       <c r="H3" s="48"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="24"/>
       <c r="E4" s="55"/>
@@ -8994,7 +8986,7 @@
       <c r="G4" s="48"/>
       <c r="H4" s="48"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="70" t="s">
         <v>17</v>
       </c>
@@ -9016,7 +9008,7 @@
         <v>Identify business objectives specifically catered towards mobile communications that are aligned to the business objectives of digital communications of your organisation.</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="70"/>
       <c r="B6" s="15" t="s">
         <v>29</v>
@@ -9036,7 +9028,7 @@
         <v>Define the types of content that are being served on mobile platforms owned by the organisation. This could include specific content types or content subject matter types.</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="70"/>
       <c r="B7" s="15" t="s">
         <v>50</v>
@@ -9056,7 +9048,7 @@
         <v>Identify KPIs for tracking the success of your mobile communications. Ensure these are based on business objectives and are specific, measurable, attainable, realistic and time-bound (SMART goals).</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="70"/>
       <c r="B8" s="16" t="s">
         <v>18</v>
@@ -9083,17 +9075,17 @@
         <v>Identify business objectives specifically catered towards mobile communications that are aligned to the business objectives of digital communications of your organisation.Define the types of content that are being served on mobile platforms owned by the organisation. This could include specific content types or content subject matter types.Identify KPIs for tracking the success of your mobile communications. Ensure these are based on business objectives and are specific, measurable, attainable, realistic and time-bound (SMART goals).</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="24"/>
     </row>
-    <row r="10" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="28"/>
       <c r="B10" s="29"/>
       <c r="C10" s="18"/>
       <c r="D10" s="30"/>
     </row>
-    <row r="11" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="70" t="s">
         <v>146</v>
       </c>
@@ -9116,7 +9108,7 @@
         <v>Evaluate the potential mobile apps offer to your digital communications. Once you make a conscious decision whether to use mobile apps, and if so how, document this in your mobile strategy.</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="70"/>
       <c r="B12" s="26" t="s">
         <v>51</v>
@@ -9137,7 +9129,7 @@
         <v>Understand how you want your mobile app(s) to support your organisational objectives.</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="70"/>
       <c r="B13" s="26" t="s">
         <v>32</v>
@@ -9158,7 +9150,7 @@
         <v>Modify your data gathering and analysis policy to include specific tracking for mobile app usage.</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="70"/>
       <c r="B14" s="15" t="s">
         <v>33</v>
@@ -9178,7 +9170,7 @@
         <v>Devise a content strategy specifically for mobile apps.</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="70"/>
       <c r="B15" s="16" t="s">
         <v>63</v>
@@ -9205,9 +9197,9 @@
         <v>Evaluate the potential mobile apps offer to your digital communications. Once you make a conscious decision whether to use mobile apps, and if so how, document this in your mobile strategy.Understand how you want your mobile app(s) to support your organisational objectives.Modify your data gathering and analysis policy to include specific tracking for mobile app usage.Devise a content strategy specifically for mobile apps.</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:20" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1"/>
+    <row r="17" spans="1:20" ht="15" customHeight="1"/>
+    <row r="18" spans="1:20" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="A18"/>
       <c r="B18" s="23"/>
       <c r="C18" s="6"/>
@@ -9229,7 +9221,7 @@
       <c r="S18"/>
       <c r="T18"/>
     </row>
-    <row r="19" spans="1:20" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="A19"/>
       <c r="B19" s="23"/>
       <c r="C19" s="6"/>
@@ -9251,7 +9243,7 @@
       <c r="S19"/>
       <c r="T19"/>
     </row>
-    <row r="20" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" s="11" customFormat="1">
       <c r="A20"/>
       <c r="B20" s="23"/>
       <c r="C20" s="6"/>
@@ -9273,7 +9265,7 @@
       <c r="S20"/>
       <c r="T20"/>
     </row>
-    <row r="21" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" s="11" customFormat="1">
       <c r="A21"/>
       <c r="B21" s="23"/>
       <c r="C21" s="6"/>
@@ -9295,7 +9287,7 @@
       <c r="S21"/>
       <c r="T21"/>
     </row>
-    <row r="22" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" s="11" customFormat="1">
       <c r="A22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="6"/>
@@ -9317,7 +9309,7 @@
       <c r="S22"/>
       <c r="T22"/>
     </row>
-    <row r="23" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" s="11" customFormat="1">
       <c r="A23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="6"/>
@@ -9339,7 +9331,7 @@
       <c r="S23"/>
       <c r="T23"/>
     </row>
-    <row r="24" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" s="11" customFormat="1">
       <c r="A24"/>
       <c r="B24" s="23"/>
       <c r="C24" s="6"/>
@@ -9361,7 +9353,7 @@
       <c r="S24"/>
       <c r="T24"/>
     </row>
-    <row r="25" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="11" customFormat="1">
       <c r="A25"/>
       <c r="B25" s="23"/>
       <c r="C25" s="6"/>
@@ -9383,7 +9375,7 @@
       <c r="S25"/>
       <c r="T25"/>
     </row>
-    <row r="26" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="11" customFormat="1">
       <c r="A26"/>
       <c r="B26" s="23"/>
       <c r="C26" s="6"/>
@@ -9405,7 +9397,7 @@
       <c r="S26"/>
       <c r="T26"/>
     </row>
-    <row r="27" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="11" customFormat="1">
       <c r="A27"/>
       <c r="B27" s="23"/>
       <c r="C27" s="6"/>
@@ -9427,7 +9419,7 @@
       <c r="S27"/>
       <c r="T27"/>
     </row>
-    <row r="28" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" s="11" customFormat="1">
       <c r="A28"/>
       <c r="B28" s="23"/>
       <c r="C28" s="6"/>
@@ -9449,7 +9441,7 @@
       <c r="S28"/>
       <c r="T28"/>
     </row>
-    <row r="29" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" s="11" customFormat="1">
       <c r="A29"/>
       <c r="B29" s="23"/>
       <c r="C29" s="6"/>
@@ -9471,7 +9463,7 @@
       <c r="S29"/>
       <c r="T29"/>
     </row>
-    <row r="30" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" s="11" customFormat="1">
       <c r="A30"/>
       <c r="B30" s="23"/>
       <c r="C30" s="6"/>
@@ -9493,7 +9485,7 @@
       <c r="S30"/>
       <c r="T30"/>
     </row>
-    <row r="31" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" s="11" customFormat="1">
       <c r="A31"/>
       <c r="B31" s="23"/>
       <c r="C31" s="6"/>
@@ -9515,7 +9507,7 @@
       <c r="S31"/>
       <c r="T31"/>
     </row>
-    <row r="32" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" s="11" customFormat="1">
       <c r="A32"/>
       <c r="B32" s="23"/>
       <c r="C32" s="6"/>
@@ -9537,7 +9529,7 @@
       <c r="S32"/>
       <c r="T32"/>
     </row>
-    <row r="33" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" s="11" customFormat="1">
       <c r="A33"/>
       <c r="B33" s="23"/>
       <c r="C33" s="6"/>
@@ -9559,7 +9551,7 @@
       <c r="S33"/>
       <c r="T33"/>
     </row>
-    <row r="34" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" s="11" customFormat="1">
       <c r="A34"/>
       <c r="B34" s="23"/>
       <c r="C34" s="6"/>
@@ -9581,7 +9573,7 @@
       <c r="S34"/>
       <c r="T34"/>
     </row>
-    <row r="35" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" s="11" customFormat="1">
       <c r="A35"/>
       <c r="B35" s="23"/>
       <c r="C35" s="6"/>
@@ -9603,7 +9595,7 @@
       <c r="S35"/>
       <c r="T35"/>
     </row>
-    <row r="36" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" s="11" customFormat="1">
       <c r="A36"/>
       <c r="B36" s="23"/>
       <c r="C36" s="6"/>
@@ -9625,7 +9617,7 @@
       <c r="S36"/>
       <c r="T36"/>
     </row>
-    <row r="37" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" s="11" customFormat="1">
       <c r="A37"/>
       <c r="B37" s="23"/>
       <c r="C37" s="6"/>
@@ -9647,7 +9639,7 @@
       <c r="S37"/>
       <c r="T37"/>
     </row>
-    <row r="38" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" s="11" customFormat="1">
       <c r="A38"/>
       <c r="B38" s="23"/>
       <c r="C38" s="6"/>
@@ -9669,7 +9661,7 @@
       <c r="S38"/>
       <c r="T38"/>
     </row>
-    <row r="39" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" s="11" customFormat="1">
       <c r="A39"/>
       <c r="B39" s="23"/>
       <c r="C39" s="6"/>
@@ -9691,7 +9683,7 @@
       <c r="S39"/>
       <c r="T39"/>
     </row>
-    <row r="40" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" s="11" customFormat="1">
       <c r="A40"/>
       <c r="B40" s="23"/>
       <c r="C40" s="6"/>
@@ -9713,7 +9705,7 @@
       <c r="S40"/>
       <c r="T40"/>
     </row>
-    <row r="41" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" s="11" customFormat="1">
       <c r="A41"/>
       <c r="B41" s="23"/>
       <c r="C41" s="6"/>
@@ -9735,7 +9727,7 @@
       <c r="S41"/>
       <c r="T41"/>
     </row>
-    <row r="42" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" s="11" customFormat="1">
       <c r="A42"/>
       <c r="B42" s="23"/>
       <c r="C42" s="6"/>
@@ -9757,7 +9749,7 @@
       <c r="S42"/>
       <c r="T42"/>
     </row>
-    <row r="43" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" s="11" customFormat="1">
       <c r="A43"/>
       <c r="B43" s="23"/>
       <c r="C43" s="6"/>
@@ -9779,7 +9771,7 @@
       <c r="S43"/>
       <c r="T43"/>
     </row>
-    <row r="44" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" s="11" customFormat="1">
       <c r="A44"/>
       <c r="B44" s="23"/>
       <c r="C44" s="6"/>
@@ -9801,7 +9793,7 @@
       <c r="S44"/>
       <c r="T44"/>
     </row>
-    <row r="45" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" s="11" customFormat="1">
       <c r="A45"/>
       <c r="B45" s="23"/>
       <c r="C45" s="6"/>
@@ -9823,7 +9815,7 @@
       <c r="S45"/>
       <c r="T45"/>
     </row>
-    <row r="46" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" s="11" customFormat="1">
       <c r="A46"/>
       <c r="B46" s="23"/>
       <c r="C46" s="6"/>
@@ -9845,7 +9837,7 @@
       <c r="S46"/>
       <c r="T46"/>
     </row>
-    <row r="47" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" s="11" customFormat="1">
       <c r="A47"/>
       <c r="B47" s="23"/>
       <c r="C47" s="6"/>
@@ -9867,7 +9859,7 @@
       <c r="S47"/>
       <c r="T47"/>
     </row>
-    <row r="48" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" s="11" customFormat="1">
       <c r="A48"/>
       <c r="B48" s="23"/>
       <c r="C48" s="6"/>
@@ -9889,7 +9881,7 @@
       <c r="S48"/>
       <c r="T48"/>
     </row>
-    <row r="49" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" s="11" customFormat="1">
       <c r="A49"/>
       <c r="B49" s="23"/>
       <c r="C49" s="6"/>
@@ -9911,7 +9903,7 @@
       <c r="S49"/>
       <c r="T49"/>
     </row>
-    <row r="50" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" s="11" customFormat="1">
       <c r="A50"/>
       <c r="B50" s="23"/>
       <c r="C50" s="6"/>
@@ -9933,7 +9925,7 @@
       <c r="S50"/>
       <c r="T50"/>
     </row>
-    <row r="51" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" s="11" customFormat="1">
       <c r="A51"/>
       <c r="B51" s="23"/>
       <c r="C51" s="6"/>
@@ -9955,7 +9947,7 @@
       <c r="S51"/>
       <c r="T51"/>
     </row>
-    <row r="52" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" s="11" customFormat="1">
       <c r="A52"/>
       <c r="B52" s="23"/>
       <c r="C52" s="6"/>
@@ -9977,7 +9969,7 @@
       <c r="S52"/>
       <c r="T52"/>
     </row>
-    <row r="53" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" s="11" customFormat="1">
       <c r="A53"/>
       <c r="B53" s="23"/>
       <c r="C53" s="6"/>
@@ -9999,7 +9991,7 @@
       <c r="S53"/>
       <c r="T53"/>
     </row>
-    <row r="54" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" s="11" customFormat="1">
       <c r="A54"/>
       <c r="B54" s="23"/>
       <c r="C54" s="6"/>
@@ -10021,7 +10013,7 @@
       <c r="S54"/>
       <c r="T54"/>
     </row>
-    <row r="55" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" s="11" customFormat="1">
       <c r="A55"/>
       <c r="B55" s="23"/>
       <c r="C55" s="6"/>
@@ -10043,7 +10035,7 @@
       <c r="S55"/>
       <c r="T55"/>
     </row>
-    <row r="56" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" s="11" customFormat="1">
       <c r="A56"/>
       <c r="B56" s="23"/>
       <c r="C56" s="6"/>
@@ -10065,7 +10057,7 @@
       <c r="S56"/>
       <c r="T56"/>
     </row>
-    <row r="57" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" s="11" customFormat="1">
       <c r="A57"/>
       <c r="B57" s="23"/>
       <c r="C57" s="6"/>
@@ -10087,7 +10079,7 @@
       <c r="S57"/>
       <c r="T57"/>
     </row>
-    <row r="58" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" s="11" customFormat="1">
       <c r="A58"/>
       <c r="B58" s="23"/>
       <c r="C58" s="6"/>
@@ -10109,7 +10101,7 @@
       <c r="S58"/>
       <c r="T58"/>
     </row>
-    <row r="59" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" s="11" customFormat="1">
       <c r="A59"/>
       <c r="B59" s="23"/>
       <c r="C59" s="6"/>
@@ -10131,7 +10123,7 @@
       <c r="S59"/>
       <c r="T59"/>
     </row>
-    <row r="60" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" s="11" customFormat="1">
       <c r="A60"/>
       <c r="B60" s="23"/>
       <c r="C60" s="6"/>
@@ -10153,7 +10145,7 @@
       <c r="S60"/>
       <c r="T60"/>
     </row>
-    <row r="61" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" s="11" customFormat="1">
       <c r="A61"/>
       <c r="B61" s="23"/>
       <c r="C61" s="6"/>
@@ -10175,7 +10167,7 @@
       <c r="S61"/>
       <c r="T61"/>
     </row>
-    <row r="62" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" s="11" customFormat="1">
       <c r="A62"/>
       <c r="B62" s="23"/>
       <c r="C62" s="6"/>
@@ -10197,7 +10189,7 @@
       <c r="S62"/>
       <c r="T62"/>
     </row>
-    <row r="63" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" s="11" customFormat="1">
       <c r="A63"/>
       <c r="B63" s="23"/>
       <c r="C63" s="6"/>
@@ -10219,7 +10211,7 @@
       <c r="S63"/>
       <c r="T63"/>
     </row>
-    <row r="64" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" s="11" customFormat="1">
       <c r="A64"/>
       <c r="B64" s="23"/>
       <c r="C64" s="6"/>
@@ -10241,7 +10233,7 @@
       <c r="S64"/>
       <c r="T64"/>
     </row>
-    <row r="65" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" s="11" customFormat="1">
       <c r="A65"/>
       <c r="B65" s="23"/>
       <c r="C65" s="6"/>
@@ -10263,7 +10255,7 @@
       <c r="S65"/>
       <c r="T65"/>
     </row>
-    <row r="66" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" s="11" customFormat="1">
       <c r="A66"/>
       <c r="B66" s="23"/>
       <c r="C66" s="6"/>
@@ -10285,7 +10277,7 @@
       <c r="S66"/>
       <c r="T66"/>
     </row>
-    <row r="67" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" s="11" customFormat="1">
       <c r="A67"/>
       <c r="B67" s="23"/>
       <c r="C67" s="6"/>
@@ -10307,7 +10299,7 @@
       <c r="S67"/>
       <c r="T67"/>
     </row>
-    <row r="68" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" s="11" customFormat="1">
       <c r="A68"/>
       <c r="B68" s="23"/>
       <c r="C68" s="6"/>
@@ -10329,7 +10321,7 @@
       <c r="S68"/>
       <c r="T68"/>
     </row>
-    <row r="69" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" s="11" customFormat="1">
       <c r="A69"/>
       <c r="B69" s="23"/>
       <c r="C69" s="6"/>
@@ -10351,7 +10343,7 @@
       <c r="S69"/>
       <c r="T69"/>
     </row>
-    <row r="70" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" s="11" customFormat="1">
       <c r="A70"/>
       <c r="B70" s="23"/>
       <c r="C70" s="6"/>
@@ -10373,7 +10365,7 @@
       <c r="S70"/>
       <c r="T70"/>
     </row>
-    <row r="71" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" s="11" customFormat="1">
       <c r="A71"/>
       <c r="B71" s="23"/>
       <c r="C71" s="6"/>
@@ -10395,7 +10387,7 @@
       <c r="S71"/>
       <c r="T71"/>
     </row>
-    <row r="72" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" s="11" customFormat="1">
       <c r="A72"/>
       <c r="B72" s="23"/>
       <c r="C72" s="6"/>
@@ -10417,7 +10409,7 @@
       <c r="S72"/>
       <c r="T72"/>
     </row>
-    <row r="73" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" s="11" customFormat="1">
       <c r="A73"/>
       <c r="B73" s="23"/>
       <c r="C73" s="6"/>
@@ -10439,7 +10431,7 @@
       <c r="S73"/>
       <c r="T73"/>
     </row>
-    <row r="74" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" s="11" customFormat="1">
       <c r="A74"/>
       <c r="B74" s="23"/>
       <c r="C74" s="6"/>
@@ -10461,7 +10453,7 @@
       <c r="S74"/>
       <c r="T74"/>
     </row>
-    <row r="75" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" s="11" customFormat="1">
       <c r="A75"/>
       <c r="B75" s="23"/>
       <c r="C75" s="6"/>
@@ -10483,7 +10475,7 @@
       <c r="S75"/>
       <c r="T75"/>
     </row>
-    <row r="76" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" s="11" customFormat="1">
       <c r="A76"/>
       <c r="B76" s="23"/>
       <c r="C76" s="6"/>
@@ -10505,7 +10497,7 @@
       <c r="S76"/>
       <c r="T76"/>
     </row>
-    <row r="77" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" s="11" customFormat="1">
       <c r="A77"/>
       <c r="B77" s="23"/>
       <c r="C77" s="6"/>
@@ -10527,7 +10519,7 @@
       <c r="S77"/>
       <c r="T77"/>
     </row>
-    <row r="78" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" s="11" customFormat="1">
       <c r="A78"/>
       <c r="B78" s="23"/>
       <c r="C78" s="6"/>
@@ -10549,7 +10541,7 @@
       <c r="S78"/>
       <c r="T78"/>
     </row>
-    <row r="79" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" s="11" customFormat="1">
       <c r="A79"/>
       <c r="B79" s="23"/>
       <c r="C79" s="6"/>
@@ -10571,7 +10563,7 @@
       <c r="S79"/>
       <c r="T79"/>
     </row>
-    <row r="80" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" s="11" customFormat="1">
       <c r="A80"/>
       <c r="B80" s="23"/>
       <c r="C80" s="6"/>
@@ -10593,7 +10585,7 @@
       <c r="S80"/>
       <c r="T80"/>
     </row>
-    <row r="81" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" s="11" customFormat="1">
       <c r="A81"/>
       <c r="B81" s="23"/>
       <c r="C81" s="6"/>
@@ -10615,7 +10607,7 @@
       <c r="S81"/>
       <c r="T81"/>
     </row>
-    <row r="82" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" s="11" customFormat="1">
       <c r="A82"/>
       <c r="B82" s="23"/>
       <c r="C82" s="6"/>
@@ -10637,7 +10629,7 @@
       <c r="S82"/>
       <c r="T82"/>
     </row>
-    <row r="83" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" s="11" customFormat="1">
       <c r="A83"/>
       <c r="B83" s="23"/>
       <c r="C83" s="6"/>
@@ -10659,7 +10651,7 @@
       <c r="S83"/>
       <c r="T83"/>
     </row>
-    <row r="84" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" s="11" customFormat="1">
       <c r="A84"/>
       <c r="B84" s="23"/>
       <c r="C84" s="6"/>
@@ -10681,7 +10673,7 @@
       <c r="S84"/>
       <c r="T84"/>
     </row>
-    <row r="85" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" s="11" customFormat="1">
       <c r="A85"/>
       <c r="B85" s="23"/>
       <c r="C85" s="6"/>
@@ -10703,7 +10695,7 @@
       <c r="S85"/>
       <c r="T85"/>
     </row>
-    <row r="86" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" s="11" customFormat="1">
       <c r="A86"/>
       <c r="B86" s="23"/>
       <c r="C86" s="6"/>
@@ -10725,7 +10717,7 @@
       <c r="S86"/>
       <c r="T86"/>
     </row>
-    <row r="87" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" s="11" customFormat="1">
       <c r="A87"/>
       <c r="B87" s="23"/>
       <c r="C87" s="6"/>
@@ -10747,7 +10739,7 @@
       <c r="S87"/>
       <c r="T87"/>
     </row>
-    <row r="88" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" s="11" customFormat="1">
       <c r="A88"/>
       <c r="B88" s="23"/>
       <c r="C88" s="6"/>
@@ -10769,7 +10761,7 @@
       <c r="S88"/>
       <c r="T88"/>
     </row>
-    <row r="89" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" s="11" customFormat="1">
       <c r="A89"/>
       <c r="B89" s="23"/>
       <c r="C89" s="6"/>
@@ -10791,7 +10783,7 @@
       <c r="S89"/>
       <c r="T89"/>
     </row>
-    <row r="90" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" s="11" customFormat="1">
       <c r="A90"/>
       <c r="B90" s="23"/>
       <c r="C90" s="6"/>
@@ -10813,7 +10805,7 @@
       <c r="S90"/>
       <c r="T90"/>
     </row>
-    <row r="91" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" s="11" customFormat="1">
       <c r="A91"/>
       <c r="B91" s="23"/>
       <c r="C91" s="6"/>
@@ -10835,7 +10827,7 @@
       <c r="S91"/>
       <c r="T91"/>
     </row>
-    <row r="92" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" s="11" customFormat="1">
       <c r="A92"/>
       <c r="B92" s="23"/>
       <c r="C92" s="6"/>
@@ -10857,7 +10849,7 @@
       <c r="S92"/>
       <c r="T92"/>
     </row>
-    <row r="93" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" s="11" customFormat="1">
       <c r="A93"/>
       <c r="B93" s="23"/>
       <c r="C93" s="6"/>
@@ -10879,7 +10871,7 @@
       <c r="S93"/>
       <c r="T93"/>
     </row>
-    <row r="94" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" s="11" customFormat="1">
       <c r="A94"/>
       <c r="B94" s="23"/>
       <c r="C94" s="6"/>
@@ -10901,7 +10893,7 @@
       <c r="S94"/>
       <c r="T94"/>
     </row>
-    <row r="95" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" s="11" customFormat="1">
       <c r="A95"/>
       <c r="B95" s="23"/>
       <c r="C95" s="6"/>
@@ -10923,7 +10915,7 @@
       <c r="S95"/>
       <c r="T95"/>
     </row>
-    <row r="96" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" s="11" customFormat="1">
       <c r="A96"/>
       <c r="B96" s="23"/>
       <c r="C96" s="6"/>
@@ -10945,7 +10937,7 @@
       <c r="S96"/>
       <c r="T96"/>
     </row>
-    <row r="97" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" s="11" customFormat="1">
       <c r="A97"/>
       <c r="B97" s="23"/>
       <c r="C97" s="6"/>
@@ -10967,7 +10959,7 @@
       <c r="S97"/>
       <c r="T97"/>
     </row>
-    <row r="98" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" s="11" customFormat="1">
       <c r="A98"/>
       <c r="B98" s="23"/>
       <c r="C98" s="6"/>
@@ -10989,7 +10981,7 @@
       <c r="S98"/>
       <c r="T98"/>
     </row>
-    <row r="99" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" s="11" customFormat="1">
       <c r="A99"/>
       <c r="B99" s="23"/>
       <c r="C99" s="6"/>
@@ -11011,7 +11003,7 @@
       <c r="S99"/>
       <c r="T99"/>
     </row>
-    <row r="100" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" s="11" customFormat="1">
       <c r="A100"/>
       <c r="B100" s="23"/>
       <c r="C100" s="6"/>
@@ -11033,7 +11025,7 @@
       <c r="S100"/>
       <c r="T100"/>
     </row>
-    <row r="101" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" s="11" customFormat="1">
       <c r="A101"/>
       <c r="B101" s="23"/>
       <c r="C101" s="6"/>
@@ -11055,7 +11047,7 @@
       <c r="S101"/>
       <c r="T101"/>
     </row>
-    <row r="102" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" s="11" customFormat="1">
       <c r="A102"/>
       <c r="B102" s="23"/>
       <c r="C102" s="6"/>
@@ -11077,7 +11069,7 @@
       <c r="S102"/>
       <c r="T102"/>
     </row>
-    <row r="103" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" s="11" customFormat="1">
       <c r="A103"/>
       <c r="B103" s="23"/>
       <c r="C103" s="6"/>
@@ -11099,7 +11091,7 @@
       <c r="S103"/>
       <c r="T103"/>
     </row>
-    <row r="104" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" s="11" customFormat="1">
       <c r="A104"/>
       <c r="B104" s="23"/>
       <c r="C104" s="6"/>
@@ -11121,7 +11113,7 @@
       <c r="S104"/>
       <c r="T104"/>
     </row>
-    <row r="105" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" s="11" customFormat="1">
       <c r="A105"/>
       <c r="B105" s="23"/>
       <c r="C105" s="6"/>
@@ -11143,7 +11135,7 @@
       <c r="S105"/>
       <c r="T105"/>
     </row>
-    <row r="106" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" s="11" customFormat="1">
       <c r="A106"/>
       <c r="B106" s="23"/>
       <c r="C106" s="6"/>
@@ -11165,7 +11157,7 @@
       <c r="S106"/>
       <c r="T106"/>
     </row>
-    <row r="107" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" s="11" customFormat="1">
       <c r="A107"/>
       <c r="B107" s="23"/>
       <c r="C107" s="6"/>
@@ -11187,7 +11179,7 @@
       <c r="S107"/>
       <c r="T107"/>
     </row>
-    <row r="108" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" s="11" customFormat="1">
       <c r="A108"/>
       <c r="B108" s="23"/>
       <c r="C108" s="6"/>
@@ -11209,7 +11201,7 @@
       <c r="S108"/>
       <c r="T108"/>
     </row>
-    <row r="109" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" s="11" customFormat="1">
       <c r="A109"/>
       <c r="B109" s="23"/>
       <c r="C109" s="6"/>
@@ -11231,7 +11223,7 @@
       <c r="S109"/>
       <c r="T109"/>
     </row>
-    <row r="110" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" s="11" customFormat="1">
       <c r="A110"/>
       <c r="B110" s="23"/>
       <c r="C110" s="6"/>
@@ -11253,7 +11245,7 @@
       <c r="S110"/>
       <c r="T110"/>
     </row>
-    <row r="111" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" s="11" customFormat="1">
       <c r="A111"/>
       <c r="B111" s="23"/>
       <c r="C111" s="6"/>
@@ -11275,7 +11267,7 @@
       <c r="S111"/>
       <c r="T111"/>
     </row>
-    <row r="112" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" s="11" customFormat="1">
       <c r="A112"/>
       <c r="B112" s="23"/>
       <c r="C112" s="6"/>
@@ -11297,7 +11289,7 @@
       <c r="S112"/>
       <c r="T112"/>
     </row>
-    <row r="113" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" s="11" customFormat="1">
       <c r="A113"/>
       <c r="B113" s="23"/>
       <c r="C113" s="6"/>
@@ -11319,7 +11311,7 @@
       <c r="S113"/>
       <c r="T113"/>
     </row>
-    <row r="114" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" s="11" customFormat="1">
       <c r="A114"/>
       <c r="B114" s="23"/>
       <c r="C114" s="6"/>
@@ -11341,7 +11333,7 @@
       <c r="S114"/>
       <c r="T114"/>
     </row>
-    <row r="115" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" s="11" customFormat="1">
       <c r="A115"/>
       <c r="B115" s="23"/>
       <c r="C115" s="6"/>
@@ -11363,7 +11355,7 @@
       <c r="S115"/>
       <c r="T115"/>
     </row>
-    <row r="116" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" s="11" customFormat="1">
       <c r="A116"/>
       <c r="B116" s="23"/>
       <c r="C116" s="6"/>
@@ -11385,7 +11377,7 @@
       <c r="S116"/>
       <c r="T116"/>
     </row>
-    <row r="117" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" s="11" customFormat="1">
       <c r="A117"/>
       <c r="B117" s="23"/>
       <c r="C117" s="6"/>
@@ -11407,7 +11399,7 @@
       <c r="S117"/>
       <c r="T117"/>
     </row>
-    <row r="118" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" s="11" customFormat="1">
       <c r="A118"/>
       <c r="B118" s="23"/>
       <c r="C118" s="6"/>
@@ -11453,7 +11445,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00ADF2"/>
   </sheetPr>
   <dimension ref="B1:M17"/>
@@ -11462,16 +11454,16 @@
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.625" customWidth="1"/>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="11.875" customWidth="1"/>
-    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" ht="47" customHeight="1">
       <c r="B1" s="72" t="s">
         <v>64</v>
       </c>
@@ -11484,16 +11476,16 @@
       <c r="G1" s="42"/>
       <c r="H1" s="42"/>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13">
       <c r="B2" t="s">
         <v>96</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" ht="45">
       <c r="B4" s="73" t="s">
         <v>35</v>
       </c>
@@ -11516,7 +11508,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13">
       <c r="B5" s="73"/>
       <c r="C5" s="9">
         <f>AVERAGE(D5:H5)</f>
@@ -11546,7 +11538,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13">
       <c r="B6" s="33"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -11560,7 +11552,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="8" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="45">
       <c r="B8" s="73" t="s">
         <v>22</v>
       </c>
@@ -11571,7 +11563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13">
       <c r="B9" s="73"/>
       <c r="C9" s="9">
         <f>D9</f>
@@ -11586,7 +11578,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13">
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="2"/>
@@ -11594,7 +11586,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="12" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="45">
       <c r="B12" s="73" t="s">
         <v>36</v>
       </c>
@@ -11612,7 +11604,7 @@
       </c>
       <c r="G12" s="33"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13">
       <c r="B13" s="73"/>
       <c r="C13" s="9">
         <f>AVERAGE(D13:F13)</f>
@@ -11635,7 +11627,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="16" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="45">
       <c r="B16" s="73" t="s">
         <v>6</v>
       </c>
@@ -11649,7 +11641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9">
       <c r="B17" s="73"/>
       <c r="C17" s="9">
         <f>AVERAGE(D17:E17)</f>
@@ -11677,7 +11669,7 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B4:B5"/>
   </mergeCells>
-  <conditionalFormatting sqref="C9 D1 J6 C5 G13 C13 C2:C3">
+  <conditionalFormatting sqref="D1 C9 J6 C5 G13 C13 C2:C3">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -11735,7 +11727,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17 C9">
+  <conditionalFormatting sqref="C9 C17">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -11761,22 +11753,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="37" customWidth="1"/>
-    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.875" style="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.625" customWidth="1"/>
-    <col min="5" max="5" width="25.875" customWidth="1"/>
-    <col min="6" max="7" width="33.375" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="37" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" customWidth="1"/>
+    <col min="6" max="7" width="33.33203125" customWidth="1"/>
     <col min="8" max="8" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="39" customFormat="1">
       <c r="A1" s="38" t="s">
         <v>69</v>
       </c>
@@ -11799,7 +11791,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -11815,7 +11807,7 @@
         <v>Assesses any written expression of strategic intent relating to digital communications the organisation has, even if it is not explicitly labelled “digital strategy”. This is based on the opinion that a digital strategy should be documented for concreteness and transferability of knowledge. Declaring a strategy is the groundwork for carrying out digital communications in a sustained manner.</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="37">
         <v>1.1000000000000001</v>
       </c>
@@ -11831,7 +11823,7 @@
         <v>Looks at elements of digital strategy that apply across channels (web, mobile, social media).</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="37" t="s">
         <v>75</v>
       </c>
@@ -11855,7 +11847,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="37" t="s">
         <v>77</v>
       </c>
@@ -11879,7 +11871,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="37" t="s">
         <v>78</v>
       </c>
@@ -11903,7 +11895,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="37" t="s">
         <v>79</v>
       </c>
@@ -11927,7 +11919,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="37" t="s">
         <v>80</v>
       </c>
@@ -11951,7 +11943,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="37">
         <v>1.2</v>
       </c>
@@ -11967,7 +11959,7 @@
         <v>Looks at elements of digital strategy that apply to the organisation’s website(s).</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="37" t="s">
         <v>85</v>
       </c>
@@ -11991,7 +11983,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="37" t="s">
         <v>86</v>
       </c>
@@ -12007,7 +11999,7 @@
         <v>Looks at elements of digital strategy that apply to the organisation’s social media engagement.</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="37" t="s">
         <v>87</v>
       </c>
@@ -12031,7 +12023,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="37" t="s">
         <v>88</v>
       </c>
@@ -12055,7 +12047,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="37" t="s">
         <v>89</v>
       </c>
@@ -12079,7 +12071,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="37" t="s">
         <v>90</v>
       </c>
@@ -12095,7 +12087,7 @@
         <v>Looks at elements of digital strategy that apply to the organisation’s mobile engagement. Even if a mobile strategy has been considered and a decision made not to engage in mobile, that decision and the reason should be documented</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="37" t="s">
         <v>91</v>
       </c>
@@ -12119,7 +12111,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="37" t="s">
         <v>93</v>
       </c>

</xml_diff>